<commit_message>
worked on preseason review
</commit_message>
<xml_diff>
--- a/refs/litreview/preseason_review.xlsx
+++ b/refs/litreview/preseason_review.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17440" yWindow="2040" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="17440" yWindow="2040" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="preseaon_review" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
   <si>
     <t>Search was: You searched for: TOPIC: (preseason  OR pre-season) AND TOPIC: (phenolog*)
 Timespan: All years. Indexes: SCI-EXPANDED, SSCI, A&amp;HCI, CPCI-S, CPCI-SSH, BKCI-S, BKCI-SSH, ESCI, CCR-EXPANDED, IC.</t>
@@ -135,6 +135,87 @@
   </si>
   <si>
     <t>pearcorr; parcorr</t>
+  </si>
+  <si>
+    <t>Huang2020</t>
+  </si>
+  <si>
+    <t>Phenological changes in herbaceous plants in ChinaÕs grasslands and their responses to climate change: a meta-analysis</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>metaanalysis with multiple preseasons in different studies</t>
+  </si>
+  <si>
+    <t>0-3 month</t>
+  </si>
+  <si>
+    <t>"The candidate previous month with the largest absolute partial correlation coefficient was finally selected as the preseason."</t>
+  </si>
+  <si>
+    <t>multiyear average Green up date</t>
+  </si>
+  <si>
+    <t>Guo2020</t>
+  </si>
+  <si>
+    <t>Impact of spring phenology variation on GPP and its lag feedback for winter wheat over the North China Plain</t>
+  </si>
+  <si>
+    <t>Yu2020</t>
+  </si>
+  <si>
+    <t>preseason Snow Water Equivalent (SWE</t>
+  </si>
+  <si>
+    <t>Forest Phenology Shifts in Response to Climate Change over China-Mongolia-Russia International Economic Corridor</t>
+  </si>
+  <si>
+    <t>Zhou2020</t>
+  </si>
+  <si>
+    <t>Assessment of varying changes of vegetation and the response to climatic factors using GIMMS NDVI3g on the Tibetan Plateau</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>Huang2020b</t>
+  </si>
+  <si>
+    <t>Effect of preseason diurnal temperature range on the start of vegetation growing season in the Northern Hemisphere</t>
+  </si>
+  <si>
+    <t>Month of Start of Spring</t>
+  </si>
+  <si>
+    <t>Candidate preseason periods were evaluated in one-month intervals working backward in time from the month of SOS to January of the current year. A partial coefficient between DTR and SOS was calculated for each candidate period, and the period with the largest partial correlation coefficient (absolute value) was selected as the preseason period. The month of SOS was determined from the multiyear average of SOS dates. If the average date was in the second half of the month, that month was chosen as the SOS month, and if the average date was in the first half of the month, the previous month was chosen.</t>
+  </si>
+  <si>
+    <t>Chai2020</t>
+  </si>
+  <si>
+    <t>The relative controls of temperature and soil moisture on the start of carbon flux phenology and net ecosystem production in two alpine meadows on the Qinghai-Tibetan Plateau</t>
+  </si>
+  <si>
+    <t>Precipitation and Minimum Temperature are Primary Climatic Controls of Alpine Grassland Autumn Phenology on the Qinghai-Tibet Plateau</t>
+  </si>
+  <si>
+    <t>An2020</t>
+  </si>
+  <si>
+    <t>autumn phenology</t>
+  </si>
+  <si>
+    <t>Change in Autumn Vegetation Phenology and the Climate Controls From 1982 to 2012 on the Qinghai-Tibet Plateau</t>
+  </si>
+  <si>
+    <t>Li2020</t>
   </si>
 </sst>
 </file>
@@ -198,8 +279,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -230,7 +313,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -242,6 +325,7 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -253,6 +337,7 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -582,13 +667,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -657,6 +742,133 @@
       </c>
       <c r="I3" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -674,7 +886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated refs help info
</commit_message>
<xml_diff>
--- a/refs/litreview/preseason_review.xlsx
+++ b/refs/litreview/preseason_review.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17440" yWindow="2040" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="19520" yWindow="0" windowWidth="23700" windowHeight="22500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="preseaon_review" sheetId="1" r:id="rId1"/>
-    <sheet name="meta" sheetId="2" r:id="rId2"/>
+    <sheet name="preseason_review" sheetId="1" r:id="rId1"/>
+    <sheet name="senswindows" sheetId="3" r:id="rId2"/>
+    <sheet name="meta" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="243">
   <si>
     <t>Search was: You searched for: TOPIC: (preseason  OR pre-season) AND TOPIC: (phenolog*)
 Timespan: All years. Indexes: SCI-EXPANDED, SSCI, A&amp;HCI, CPCI-S, CPCI-SSH, BKCI-S, BKCI-SSH, ESCI, CCR-EXPANDED, IC.</t>
@@ -140,9 +141,6 @@
     <t>Huang2020</t>
   </si>
   <si>
-    <t>Phenological changes in herbaceous plants in ChinaÕs grasslands and their responses to climate change: a meta-analysis</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -216,13 +214,550 @@
   </si>
   <si>
     <t>Li2020</t>
+  </si>
+  <si>
+    <t>ISI_authors</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>assigned</t>
+  </si>
+  <si>
+    <t>Yuan, MX; Zhao, L; Lin, AW; Wang, LC; Li, QJ; She, DX; Qu, S</t>
+  </si>
+  <si>
+    <t>Chen, XH; Wang, WQ; Chen, J; Zhu, XL; Shen, MG; Gan, LQ; Cao, X</t>
+  </si>
+  <si>
+    <t>Huang, WJ; Dai, JH; Wang, W; Li, JS; Feng, CT; Du, JH</t>
+  </si>
+  <si>
+    <t>Guo, LH; Gao, JB; Ma, SC; Chang, Q; Zhang, LL; Wang, SX; Zou, YF; Wu, SH; Xiao, XM</t>
+  </si>
+  <si>
+    <t>Yu, LX; Yan, ZR; Zhang, SW</t>
+  </si>
+  <si>
+    <t>Zhou, YK; Fan, JF; Wang, XY</t>
+  </si>
+  <si>
+    <t>Huang, Y; Jiang, N; Shen, MG; Guo, L</t>
+  </si>
+  <si>
+    <t>Chai, X; Shi, PL; Song, MH; Zong, N; He, YT; Li, YN; Zhang, XZ; Liu, YJ</t>
+  </si>
+  <si>
+    <t>An, S; Chen, XQ; Zhang, XY; Lang, WG; Ren, SL; Xu, L</t>
+  </si>
+  <si>
+    <t>Li, P; Zhu, QA; Peng, CH; Zhang, J; Wang, M; Zhang, JJ; Ding, JH; Zhou, XL</t>
+  </si>
+  <si>
+    <t>Yuan, MX; Wang, LC; Lin, AW; Liu, ZJ; Li, QJ; Qu, S</t>
+  </si>
+  <si>
+    <t>Dai, WJ; Jin, HY; Zhang, YH; Liu, T; Zhou, ZQ</t>
+  </si>
+  <si>
+    <t>Deng, HY; Yin, YH; Wu, SH; Xu, XF</t>
+  </si>
+  <si>
+    <t>Wu, XF; Yang, W; Wang, CY; Shen, YJ; Kondoh, A</t>
+  </si>
+  <si>
+    <t>Ghosh, S; Nandy, S; Mohanty, S; Subba, R; Kushwaha, SPS</t>
+  </si>
+  <si>
+    <t>Wang, XY; Wu, CY</t>
+  </si>
+  <si>
+    <t>Du, J; Li, K; He, ZB; Chen, LF; Lin, PF; Zhu, X</t>
+  </si>
+  <si>
+    <t>Xia, HM; Qin, YC; Feng, G; Meng, QM; Cui, YP; Song, HQ; Ouyang, Y; Liu, GJ</t>
+  </si>
+  <si>
+    <t>Yang, JL; Dong, JW; Xiao, XM; Dai, JH; Wu, CY; Xia, JY; Zhao, GS; Zhao, MM; Li, ZL; Zhang, Y; Ge, QS</t>
+  </si>
+  <si>
+    <t>Ren, SL; Qin, QM; Ren, HZ; Sui, J; Zhang, Y</t>
+  </si>
+  <si>
+    <t>Wang, GC; Huang, Y; Wei, YR; Zhang, W; Li, TT; Zhang, Q</t>
+  </si>
+  <si>
+    <t>Yuan, MX; Wang, LC; Lin, AW; Liu, ZJ; Qu, S</t>
+  </si>
+  <si>
+    <t>Deng, GR; Zhang, HY; Guo, XY; Shan, Y; Ying, H; Wu, RH; Li, H; Han, YL</t>
+  </si>
+  <si>
+    <t>Guo, LH; Gao, JB; Hao, CY; Zhang, LL; Wu, SH; Xiao, XM</t>
+  </si>
+  <si>
+    <t>Meng, FD; Zhang, LR; Zhang, ZH; Jiang, LL; Wang, YF; Duan, JC; Wang, Q; Li, BW; Liu, PP; Hong, H; Lv, WW; Renzeng, WM; Wang, ZZ; Luo, CY; Dorj, T; Zhou, HK; Du, MY; Wang, SP</t>
+  </si>
+  <si>
+    <t>Huang, K; Zu, JX; Zhang, YJ; Cong, N; Liu, YJ; Chen, N</t>
+  </si>
+  <si>
+    <t>Du, J; He, ZB; Piatek, KB; Chen, LF; Lin, PF; Zhu, X</t>
+  </si>
+  <si>
+    <t>Ren, SL; Qin, QM; Ren, HZ</t>
+  </si>
+  <si>
+    <t>Wang, HJ; Zhong, SY; Tao, ZX; Dai, JH; Ge, QS</t>
+  </si>
+  <si>
+    <t>Dai, JH; Xu, YJ; Wang, HJ; Alatalo, J; Tao, ZX; Ge, QS</t>
+  </si>
+  <si>
+    <t>Liu, D; Wang, T; Yang, T; Yan, ZJ; Liu, YW; Zhao, YT; Piao, SL</t>
+  </si>
+  <si>
+    <t>Wang, HL; Tetzlaff, D; Buttle, J; Carey, SK; Laudon, H; McNamara, JP; Spence, C; Soulsby, C</t>
+  </si>
+  <si>
+    <t>Wang, J; Wu, CY; Wang, XY; Zhang, XY</t>
+  </si>
+  <si>
+    <t>Qiao, DJ; Zhou, JM; Liang, S; Fu, XY</t>
+  </si>
+  <si>
+    <t>Wu, CY; Wang, XY; Wang, HJ; Ciais, P; Penuelas, J; Myneni, RB; Desai, AR; Gough, CM; Gonsamo, A; Black, AT; Jassal, RS; Ju, WM; Yuan, WP; Fu, YS; Shen, MG; Li, SH; Liu, RG; Chen, JM; Ge, QS</t>
+  </si>
+  <si>
+    <t>Xu, YJ; Wang, HJ; Ge, QS; Wu, CY; Dai, JH</t>
+  </si>
+  <si>
+    <t>Yun, J; Jeong, SJ; Ho, CH; Park, CE; Park, H; Kim, J</t>
+  </si>
+  <si>
+    <t>Park, H; Jeong, SJ; Ho, CH; Park, CE; Kim, J</t>
+  </si>
+  <si>
+    <t>Ma, QQ; Huang, JG; Hanninen, H; Berninger, F</t>
+  </si>
+  <si>
+    <t>Asse, D; Chuine, I; Vitasse, Y; Yoccoz, NG; Delpierre, N; Badeau, V; Delestrade, A; Randin, CF</t>
+  </si>
+  <si>
+    <t>Fu, YY; He, HS; Zhao, JJ; Larsen, DR; Zhang, HY; Sunde, MG; Duan, SW</t>
+  </si>
+  <si>
+    <t>Cheng, M; Jin, JX; Zhang, JM; Jiang, H; Wang, RZ</t>
+  </si>
+  <si>
+    <t>Ren, SL; Yi, SH; Peichl, M; Wang, XY</t>
+  </si>
+  <si>
+    <t>Xu, XY; Riley, WJ; Koven, CD; Jia, GS</t>
+  </si>
+  <si>
+    <t>Yang, ZY; Shen, MG; Jia, SG; Guo, L; Yang, W; Wang, C; Chen, XH; Chen, J</t>
+  </si>
+  <si>
+    <t>Gusewell, S; Furrer, R; Gehrig, R; Pietragalla, B</t>
+  </si>
+  <si>
+    <t>Cong, N; Shen, MG; Piao, SL</t>
+  </si>
+  <si>
+    <t>Zhu, WQ; Jiang, N; Chen, GS; Zhang, DH; Zheng, ZT; Fan, DQ</t>
+  </si>
+  <si>
+    <t>Wang, SS; Mo, XG; Liu, ZJ; Baig, MHA; Chi, WF</t>
+  </si>
+  <si>
+    <t>Tao, ZX; Wang, HJ; Liu, YC; Xu, YJ; Dai, JH</t>
+  </si>
+  <si>
+    <t>Liu, Q; Fu, YSH; Zhu, ZC; Liu, YW; Liu, Z; Huang, MT; Janssens, IA; Piao, SL</t>
+  </si>
+  <si>
+    <t>Nguy-Robertson, AL; Zygielbaum, AI; McMechan, AJ; Hein, GL; Wegulo, SN; Stilwell, AR; Smith, TM</t>
+  </si>
+  <si>
+    <t>Shen, MG; Piao, SL; Chen, XQ; An, S; Fu, YSH; Wang, SP; Cong, N; Janssens, IA</t>
+  </si>
+  <si>
+    <t>Sha, ZY; Zhong, JL; Bai, YF; Tan, XC; Li, J</t>
+  </si>
+  <si>
+    <t>Ge, QS; Dai, JH; Cui, HJ; Wang, HJ</t>
+  </si>
+  <si>
+    <t>Liu, Q; Fu, YSH; Zeng, ZZ; Huang, MT; Li, XR; Piao, SL</t>
+  </si>
+  <si>
+    <t>Shen, MG; Piao, SL; Dorji, T; Liu, Q; Cong, N; Chen, XQ; An, S; Wang, SP; Wang, T; Zhang, GX</t>
+  </si>
+  <si>
+    <t>Chen, XQ; An, S; Inouye, DW; Schwartz, MD</t>
+  </si>
+  <si>
+    <t>Shen, MG; Piao, SL; Cong, N; Zhang, GX; Janssens, IA</t>
+  </si>
+  <si>
+    <t>Zhu, LK; Southworth, J; Meng, JJ</t>
+  </si>
+  <si>
+    <t>Shen, MG; Cong, N; Cao, RY</t>
+  </si>
+  <si>
+    <t>Wang, HJ; Ge, QS; Dai, JH; Tao, ZX</t>
+  </si>
+  <si>
+    <t>Wang, C; Cao, RY; Chen, J; Rao, YH; Tang, YH</t>
+  </si>
+  <si>
+    <t>Yang, YT; Guan, HD; Shen, MG; Liang, W; Jiang, L</t>
+  </si>
+  <si>
+    <t>Tang, G; Arnone, JA; Verburg, PSJ; Jasoni, RL; Sun, L</t>
+  </si>
+  <si>
+    <t>Asilo, S; de Bie, K; Skidmore, A; Nelson, A; Barbieri, M; Maunahan, A</t>
+  </si>
+  <si>
+    <t>Shen, MG; Tang, YH; Chen, J; Yang, X; Wang, C; Cui, XY; Yang, YP; Han, LJ; Li, L; Du, JH; Zhang, GX; Cong, N</t>
+  </si>
+  <si>
+    <t>Xia, HM; Li, AN; Zhao, W; Jin, HA; Lei, GB; Bian, JH; Tan, JB</t>
+  </si>
+  <si>
+    <t>Wainwright, CE; Wolkovich, EM; Cleland, EE</t>
+  </si>
+  <si>
+    <t>Shen, MG; Tang, YH; Chen, J; Zhu, XL; Zheng, YH</t>
+  </si>
+  <si>
+    <t>Jeong, SJ; Ho, CH; Gim, HJ; Brown, ME</t>
+  </si>
+  <si>
+    <t>Ko, JH; Piccinni, G; Steglich, E</t>
+  </si>
+  <si>
+    <t>Yli-Panula, E; Fekedulegn, DB; Green, BJ; Ranta, H</t>
+  </si>
+  <si>
+    <t>Tao, F; Yokozawa, M; Zhang, Z; Hayashi, Y; Ishigooka, Y</t>
+  </si>
+  <si>
+    <t>Skjoth, CA; Sommer, J; Stach, A; Smith, M; Brandt, J</t>
+  </si>
+  <si>
+    <t>Berger, JD; Ali, M; Basu, PS; Chaudhary, BD; Chaturvedi, SK; Deshmukh, PS; Dharmaraj, PS; Dwivedi, SK; Gangadhar, GC; Gaur, PM; Kumar, J; Pannu, RK; Siddique, KHM; Singh, DN; Singh, DR; Singh, SJ; Turner, NC; Yadava, HS; Yadav, SS</t>
+  </si>
+  <si>
+    <t>Phenological changes in herbaceous plants in China's grasslands and their responses to climate change: a meta-analysis</t>
+  </si>
+  <si>
+    <t>Vegetation green up under the influence of daily minimum temperature and urbanization in the Yellow River Basin, China</t>
+  </si>
+  <si>
+    <t>Detecting temporal changes in the temperature sensitivity of spring phenology with global warming: Application of machine learning in phenological model</t>
+  </si>
+  <si>
+    <t>Contrasting drought impacts on the start of phenological growing season in Northern China during 1982-2015</t>
+  </si>
+  <si>
+    <t>Interactions among the Phenological Events of Winter Wheat in the North China Plain-Based on Field Data and Improved MODIS Estimation</t>
+  </si>
+  <si>
+    <t>Are phenological variations in natural teak (Tectona grandis) forests of India governed by rainfall? A remote sensing based investigation</t>
+  </si>
+  <si>
+    <t>Estimating the peak of growing season (POS) of China's terrestrial ecosystems</t>
+  </si>
+  <si>
+    <t>Daily minimum temperature and precipitation control on spring phenology in arid-mountain ecosystems in China</t>
+  </si>
+  <si>
+    <t>Forest Phenology Dynamics to Climate Change and Topography in a Geographic and Climate Transition Zone: The Qinling Mountains in Central China</t>
+  </si>
+  <si>
+    <t>Divergent shifts in peak photosynthesis timing of temperate and alpine grasslands in China</t>
+  </si>
+  <si>
+    <t>New model for simulating autumn phenology of herbaceous plants in the Inner Mongolian Grassland</t>
+  </si>
+  <si>
+    <t>Inner Mongolian grassland plant phenological changes and their climatic drivers</t>
+  </si>
+  <si>
+    <t>Variations in land surface phenology and their response to climate change in Yangtze River basin during 1982-2015</t>
+  </si>
+  <si>
+    <t>Asymmetric Effects of Daytime and Nighttime Warming on Boreal Forest Spring Phenology</t>
+  </si>
+  <si>
+    <t>Winter Wheat Green-up Date Variation and its Diverse Response on the Hydrothermal Conditions over the North China Plain, Using MODIS Time-Series Data</t>
+  </si>
+  <si>
+    <t>Opposite effects of winter day and night temperature changes on early phenophases</t>
+  </si>
+  <si>
+    <t>Impacts of snow cover duration on vegetation spring phenology over the Tibetan Plateau</t>
+  </si>
+  <si>
+    <t>Interacting effects of temperature and precipitation on climatic sensitivity of spring vegetation green-up in arid mountains of China</t>
+  </si>
+  <si>
+    <t>Contrasting wheat phenological responses to climate change in global scale</t>
+  </si>
+  <si>
+    <t>Changes in flowering phenology of woody plants from 1963 to 2014 in North China</t>
+  </si>
+  <si>
+    <t>Variations in the temperature sensitivity of spring leaf phenology from 1978 to 2014 in Mudanjiang, China</t>
+  </si>
+  <si>
+    <t>Deciphering impacts of climate extremes on Tibetan grasslands in the last fifteen years</t>
+  </si>
+  <si>
+    <t>Heat and Drought Stress Advanced Global Wheat Harvest Timing from 1981-2014</t>
+  </si>
+  <si>
+    <t>Climate-phenology-hydrology interactions in northern high latitudes: Assessing the value of remote sensing data in catchment ecohydrological studies</t>
+  </si>
+  <si>
+    <t>A new algorithm for the estimation of leaf unfolding date using MODIS data over China's terrestrial ecosystems</t>
+  </si>
+  <si>
+    <t>Combined Effects of Precipitation and Temperature on the Responses of Forest Spring Phenology to Winter Snow Cover Dynamics in Northeast China</t>
+  </si>
+  <si>
+    <t>Contrasting responses of autumn-leaf senescence to daytime and night-time warming</t>
+  </si>
+  <si>
+    <t>The strength of flowering-temperature relationship and preseason length affect temperature sensitivity of first flowering date across space</t>
+  </si>
+  <si>
+    <t>Influence of winter precipitation on spring phenology in boreal forests</t>
+  </si>
+  <si>
+    <t>Slowdown of spring green-up advancements in boreal forests</t>
+  </si>
+  <si>
+    <t>Reduced geographical variability in spring phenology of temperate trees with recent warming</t>
+  </si>
+  <si>
+    <t>Warmer winters reduce the advance of tree spring phenology induced by warmer springs in the Alps</t>
+  </si>
+  <si>
+    <t>Climate and Spring Phenology Effects on Autumn Phenology in the Greater Khingan Mountains, Northeastern China</t>
+  </si>
+  <si>
+    <t>Effect of climate change on vegetation phenology of different land-cover types on the Tibetan Plateau</t>
+  </si>
+  <si>
+    <t>Diverse Responses of Vegetation Phenology to Climate Change in Different Grasslands in Inner Mongolia during 2000-2016</t>
+  </si>
+  <si>
+    <t>Observed and Simulated Sensitivities of Spring Greenup to Preseason Climate in Northern Temperate and Boreal Regions</t>
+  </si>
+  <si>
+    <t>Asymmetric Responses of the End of Growing Season to Daily Maximum and Minimum Temperatures on the Tibetan Plateau</t>
+  </si>
+  <si>
+    <t>Changes in temperature sensitivity of spring phenology with recent climate warming in Switzerland are related to shifts of the preseason</t>
+  </si>
+  <si>
+    <t>Spatial variations in responses of vegetation autumn phenology to climate change on the Tibetan Plateau</t>
+  </si>
+  <si>
+    <t>Divergent shifts and responses of plant autumn phenology to climate change on the Qinghai-Tibetan Plateau</t>
+  </si>
+  <si>
+    <t>Understanding long-term (1982-2013) patterns and trends in winter wheat spring green-up date over the North China Plain</t>
+  </si>
+  <si>
+    <t>Phenological response of different vegetation types to temperature and precipitation variations in northern China during 1982-2012</t>
+  </si>
+  <si>
+    <t>Delayed autumn phenology in the Northern Hemisphere is related to change in both climate and spring phenology</t>
+  </si>
+  <si>
+    <t>Developing the framework for a risk map for mite vectored viruses in wheat resulting from pre-harvest hail damage</t>
+  </si>
+  <si>
+    <t>Strong impacts of daily minimum temperature on the green-up date and summer greenness of the Tibetan Plateau</t>
+  </si>
+  <si>
+    <t>Spatio-temporal patterns of satellite-derived grassland vegetation phenology from 1998 to 2012 in Inner Mongolia, China</t>
+  </si>
+  <si>
+    <t>Spatiotemporal Variability in Start and End of Growing Season in China Related to Climate Variability</t>
+  </si>
+  <si>
+    <t>Temperature, precipitation, and insolation effects on autumn vegetation phenology in temperate China</t>
+  </si>
+  <si>
+    <t>Plant phenological responses to climate change on the Tibetan Plateau: research status and challenges</t>
+  </si>
+  <si>
+    <t>Temperature and snowfall trigger alpine vegetation green-up on the world's roof</t>
+  </si>
+  <si>
+    <t>Precipitation impacts on vegetation spring phenology on the Tibetan Plateau</t>
+  </si>
+  <si>
+    <t>Comparison of the driving forces of spring phenology among savanna landscapes by including combined spatial and temporal heterogeneity</t>
+  </si>
+  <si>
+    <t>Temperature sensitivity as an explanation of the latitudinal pattern of green-up date trend in Northern Hemisphere vegetation during 1982-2008</t>
+  </si>
+  <si>
+    <t>Geographical pattern in first bloom variability and its relation to temperature sensitivity in the USA and China</t>
+  </si>
+  <si>
+    <t>Temperature sensitivity of spring vegetation phenology correlates to within-spring warming speed over the Northern Hemisphere</t>
+  </si>
+  <si>
+    <t>Changes in autumn vegetation dormancy onset date and the climate controls across temperate ecosystems in China from 1982 to 2010</t>
+  </si>
+  <si>
+    <t>Trends and climatic sensitivities of vegetation phenology in semiarid and arid ecosystems in the US Great Basin during 1982-2011</t>
+  </si>
+  <si>
+    <t>Complementarity of Two Rice Mapping Approaches: Characterizing Strata Mapped by Hypertemporal MODIS and Rice Paddy Identification Using Multitemporal SAR</t>
+  </si>
+  <si>
+    <t>Earlier-Season Vegetation Has Greater Temperature Sensitivity of Spring Phenology in Northern Hemisphere</t>
+  </si>
+  <si>
+    <t>SPATIO-TEMPORAL VARIATION AND DRIVING FORCES IN ALPINE GRASSLAND PHENOLOGY IN THE ZOIGE PLATEAU FROM 2001-2013</t>
+  </si>
+  <si>
+    <t>Seasonal priority effects: implications for invasion and restoration in a semi-arid system</t>
+  </si>
+  <si>
+    <t>Influences of temperature and precipitation before the growing season on spring phenology in grasslands of the central and eastern Qinghai-Tibetan Plateau</t>
+  </si>
+  <si>
+    <t>Phenology shifts at start vs. end of growing season in temperate vegetation over the Northern Hemisphere for the period 1982-2008</t>
+  </si>
+  <si>
+    <t>Using EPIC model to manage irrigated cotton and maize</t>
+  </si>
+  <si>
+    <t>Analysis of Airborne Betula Pollen in Finland; a 31-Year Perspective</t>
+  </si>
+  <si>
+    <t>Land surface phenology dynamics and climate variations in the North East China Transect (NECT), 1982-2000</t>
+  </si>
+  <si>
+    <t>The long-range transport of birch (Betula) pollen from Poland and Germany causes significant pre-season concentrations in Denmark</t>
+  </si>
+  <si>
+    <t>Genotype by environment studies demonstrate the critical role of phenology in adaptation of chickpea (Cicer arietinum L.) to high and low yielding environments of India</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>DMB</t>
+  </si>
+  <si>
+    <t>AKE</t>
+  </si>
+  <si>
+    <t>IMC</t>
+  </si>
+  <si>
+    <t>Below about preseason_review:</t>
+  </si>
+  <si>
+    <t>Below about senswindows:</t>
+  </si>
+  <si>
+    <t>who_entered</t>
+  </si>
+  <si>
+    <t>firstauthor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The goal of this is to list papers we know of that calculated sensitivity and note how they did it. </t>
+  </si>
+  <si>
+    <t>Ideally these are papers NOT picked up in the pre-season review above.</t>
+  </si>
+  <si>
+    <t>On 2 Sep 2020 Lizzie wrote:</t>
+  </si>
+  <si>
+    <t>your initials</t>
+  </si>
+  <si>
+    <t>first author of paper</t>
+  </si>
+  <si>
+    <t>year of paper</t>
+  </si>
+  <si>
+    <t>if they used another window, add info here</t>
+  </si>
+  <si>
+    <t>sens_window_howchosen</t>
+  </si>
+  <si>
+    <t>statistical_search OR pre-chosen</t>
+  </si>
+  <si>
+    <t>what was their window? See categories below</t>
+  </si>
+  <si>
+    <t>sens_window_info</t>
+  </si>
+  <si>
+    <t>sens_window_alt_info</t>
+  </si>
+  <si>
+    <t>Categories for sens_window_howchosen:</t>
+  </si>
+  <si>
+    <t>Categories for sens_window_info:</t>
+  </si>
+  <si>
+    <t>statisticalsearch</t>
+  </si>
+  <si>
+    <t>predefined</t>
+  </si>
+  <si>
+    <t>EMW</t>
+  </si>
+  <si>
+    <t>Cook</t>
+  </si>
+  <si>
+    <t>Wolkovich</t>
+  </si>
+  <si>
+    <t>MAT</t>
+  </si>
+  <si>
+    <t>supp tried many more</t>
+  </si>
+  <si>
+    <t>Warming experiments underpredict plant phenological responses to climate change</t>
+  </si>
+  <si>
+    <t>Divergent responses to spring and winter warming drive community level flowering trends</t>
+  </si>
+  <si>
+    <t>3-mo moving windows beginning the previous fall and ending at the end of the concurrent year, mean daily temperatures were compiled into seasonal growing degree day (GDD) summations and standardized to Z-score values (zero mean, unit SD)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -261,6 +796,21 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -279,7 +829,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -305,15 +855,55 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -326,6 +916,25 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -338,6 +947,25 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -667,208 +1295,1245 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:L78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2">
+        <v>2020</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>22</v>
       </c>
       <c r="B3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3">
+        <v>2020</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="4">
+      <c r="I3" s="4">
         <v>43831</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>28</v>
       </c>
-      <c r="I3" t="s">
+      <c r="L3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>38</v>
       </c>
       <c r="B4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5">
+        <v>2020</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
         <v>39</v>
       </c>
-      <c r="C4" t="s">
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6">
+        <v>2020</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7">
+        <v>2020</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8">
+        <v>2020</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" t="s">
         <v>34</v>
       </c>
-      <c r="F5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="I8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>212</v>
+      </c>
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9">
+        <v>2020</v>
+      </c>
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10">
+        <v>2020</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
+      <c r="G10" t="s">
         <v>61</v>
       </c>
-      <c r="B10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" t="s">
+        <v>212</v>
+      </c>
+      <c r="C11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11">
+        <v>2020</v>
+      </c>
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s">
-        <v>62</v>
+      <c r="G11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="B12" t="s">
+        <v>212</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12">
+        <v>2020</v>
+      </c>
+      <c r="E12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="B13" t="s">
+        <v>212</v>
+      </c>
+      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13">
+        <v>2019</v>
+      </c>
+      <c r="E13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="B14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14">
+        <v>2020</v>
+      </c>
+      <c r="E14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="B15" t="s">
+        <v>212</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15">
+        <v>2019</v>
+      </c>
+      <c r="E15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="B16" t="s">
+        <v>212</v>
+      </c>
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16">
+        <v>2019</v>
+      </c>
+      <c r="E16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" t="s">
+        <v>212</v>
+      </c>
+      <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17">
+        <v>2019</v>
+      </c>
+      <c r="E17" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" t="s">
+        <v>212</v>
+      </c>
+      <c r="C18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18">
+        <v>2020</v>
+      </c>
+      <c r="E18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" t="s">
+        <v>212</v>
+      </c>
+      <c r="C19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19">
+        <v>2019</v>
+      </c>
+      <c r="E19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" t="s">
+        <v>212</v>
+      </c>
+      <c r="C20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20">
+        <v>2019</v>
+      </c>
+      <c r="E20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" t="s">
+        <v>212</v>
+      </c>
+      <c r="C21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21">
+        <v>2019</v>
+      </c>
+      <c r="E21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22">
+        <v>2019</v>
+      </c>
+      <c r="E22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" t="s">
+        <v>212</v>
+      </c>
+      <c r="C23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23">
+        <v>2019</v>
+      </c>
+      <c r="E23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" t="s">
+        <v>212</v>
+      </c>
+      <c r="C24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24">
+        <v>2019</v>
+      </c>
+      <c r="E24" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" t="s">
+        <v>212</v>
+      </c>
+      <c r="C25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25">
+        <v>2019</v>
+      </c>
+      <c r="E25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" t="s">
+        <v>212</v>
+      </c>
+      <c r="C26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26">
+        <v>2019</v>
+      </c>
+      <c r="E26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" t="s">
+        <v>212</v>
+      </c>
+      <c r="C27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27">
+        <v>2019</v>
+      </c>
+      <c r="E27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" t="s">
+        <v>213</v>
+      </c>
+      <c r="C28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28">
+        <v>2019</v>
+      </c>
+      <c r="E28" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" t="s">
+        <v>213</v>
+      </c>
+      <c r="C29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29">
+        <v>2019</v>
+      </c>
+      <c r="E29" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30" t="s">
+        <v>213</v>
+      </c>
+      <c r="C30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30">
+        <v>2019</v>
+      </c>
+      <c r="E30" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31">
+        <v>2019</v>
+      </c>
+      <c r="E31" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" t="s">
+        <v>213</v>
+      </c>
+      <c r="C32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32">
+        <v>2019</v>
+      </c>
+      <c r="E32" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" t="s">
+        <v>213</v>
+      </c>
+      <c r="C33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33">
+        <v>2019</v>
+      </c>
+      <c r="E33" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" t="s">
+        <v>213</v>
+      </c>
+      <c r="C34" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34">
+        <v>2019</v>
+      </c>
+      <c r="E34" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" t="s">
+        <v>213</v>
+      </c>
+      <c r="C35" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35">
+        <v>2019</v>
+      </c>
+      <c r="E35" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="B36" t="s">
+        <v>213</v>
+      </c>
+      <c r="C36" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36">
+        <v>2019</v>
+      </c>
+      <c r="E36" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="B37" t="s">
+        <v>213</v>
+      </c>
+      <c r="C37" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37">
+        <v>2018</v>
+      </c>
+      <c r="E37" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="B38" t="s">
+        <v>213</v>
+      </c>
+      <c r="C38" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38">
+        <v>2018</v>
+      </c>
+      <c r="E38" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="B39" t="s">
+        <v>213</v>
+      </c>
+      <c r="C39" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39">
+        <v>2018</v>
+      </c>
+      <c r="E39" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="B40" t="s">
+        <v>213</v>
+      </c>
+      <c r="C40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40">
+        <v>2018</v>
+      </c>
+      <c r="E40" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="B41" t="s">
+        <v>213</v>
+      </c>
+      <c r="C41" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41">
+        <v>2018</v>
+      </c>
+      <c r="E41" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="B42" t="s">
+        <v>213</v>
+      </c>
+      <c r="C42" t="s">
+        <v>106</v>
+      </c>
+      <c r="D42">
+        <v>2018</v>
+      </c>
+      <c r="E42" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="B43" t="s">
+        <v>213</v>
+      </c>
+      <c r="C43" t="s">
+        <v>107</v>
+      </c>
+      <c r="D43">
+        <v>2018</v>
+      </c>
+      <c r="E43" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="B44" t="s">
+        <v>213</v>
+      </c>
+      <c r="C44" t="s">
+        <v>108</v>
+      </c>
+      <c r="D44">
+        <v>2018</v>
+      </c>
+      <c r="E44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="B45" t="s">
+        <v>213</v>
+      </c>
+      <c r="C45" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45">
+        <v>2018</v>
+      </c>
+      <c r="E45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5">
+      <c r="B46" t="s">
+        <v>213</v>
+      </c>
+      <c r="C46" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46">
+        <v>2018</v>
+      </c>
+      <c r="E46" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5">
+      <c r="B47" t="s">
+        <v>213</v>
+      </c>
+      <c r="C47" t="s">
+        <v>111</v>
+      </c>
+      <c r="D47">
+        <v>2017</v>
+      </c>
+      <c r="E47" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5">
+      <c r="B48" t="s">
+        <v>213</v>
+      </c>
+      <c r="C48" t="s">
+        <v>112</v>
+      </c>
+      <c r="D48">
+        <v>2017</v>
+      </c>
+      <c r="E48" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5">
+      <c r="B49" t="s">
+        <v>213</v>
+      </c>
+      <c r="C49" t="s">
+        <v>113</v>
+      </c>
+      <c r="D49">
+        <v>2017</v>
+      </c>
+      <c r="E49" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5">
+      <c r="B50" t="s">
+        <v>213</v>
+      </c>
+      <c r="C50" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50">
+        <v>2017</v>
+      </c>
+      <c r="E50" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5">
+      <c r="B51" t="s">
+        <v>213</v>
+      </c>
+      <c r="C51" t="s">
+        <v>115</v>
+      </c>
+      <c r="D51">
+        <v>2017</v>
+      </c>
+      <c r="E51" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5">
+      <c r="B52" t="s">
+        <v>213</v>
+      </c>
+      <c r="C52" t="s">
+        <v>116</v>
+      </c>
+      <c r="D52">
+        <v>2017</v>
+      </c>
+      <c r="E52" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5">
+      <c r="B53" t="s">
+        <v>214</v>
+      </c>
+      <c r="C53" t="s">
+        <v>117</v>
+      </c>
+      <c r="D53">
+        <v>2016</v>
+      </c>
+      <c r="E53" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5">
+      <c r="B54" t="s">
+        <v>214</v>
+      </c>
+      <c r="C54" t="s">
+        <v>118</v>
+      </c>
+      <c r="D54">
+        <v>2016</v>
+      </c>
+      <c r="E54" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5">
+      <c r="B55" t="s">
+        <v>214</v>
+      </c>
+      <c r="C55" t="s">
+        <v>119</v>
+      </c>
+      <c r="D55">
+        <v>2016</v>
+      </c>
+      <c r="E55" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5">
+      <c r="B56" t="s">
+        <v>214</v>
+      </c>
+      <c r="C56" t="s">
+        <v>120</v>
+      </c>
+      <c r="D56">
+        <v>2016</v>
+      </c>
+      <c r="E56" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5">
+      <c r="B57" t="s">
+        <v>214</v>
+      </c>
+      <c r="C57" t="s">
+        <v>121</v>
+      </c>
+      <c r="D57">
+        <v>2016</v>
+      </c>
+      <c r="E57" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5">
+      <c r="B58" t="s">
+        <v>214</v>
+      </c>
+      <c r="C58" t="s">
+        <v>122</v>
+      </c>
+      <c r="D58">
+        <v>2016</v>
+      </c>
+      <c r="E58" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5">
+      <c r="B59" t="s">
+        <v>214</v>
+      </c>
+      <c r="C59" t="s">
+        <v>123</v>
+      </c>
+      <c r="D59">
+        <v>2015</v>
+      </c>
+      <c r="E59" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5">
+      <c r="B60" t="s">
+        <v>214</v>
+      </c>
+      <c r="C60" t="s">
+        <v>124</v>
+      </c>
+      <c r="D60">
+        <v>2015</v>
+      </c>
+      <c r="E60" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5">
+      <c r="B61" t="s">
+        <v>214</v>
+      </c>
+      <c r="C61" t="s">
+        <v>125</v>
+      </c>
+      <c r="D61">
+        <v>2015</v>
+      </c>
+      <c r="E61" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5">
+      <c r="B62" t="s">
+        <v>214</v>
+      </c>
+      <c r="C62" t="s">
+        <v>126</v>
+      </c>
+      <c r="D62">
+        <v>2015</v>
+      </c>
+      <c r="E62" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5">
+      <c r="B63" t="s">
+        <v>214</v>
+      </c>
+      <c r="C63" t="s">
+        <v>127</v>
+      </c>
+      <c r="D63">
+        <v>2015</v>
+      </c>
+      <c r="E63" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5">
+      <c r="B64" t="s">
+        <v>214</v>
+      </c>
+      <c r="C64" t="s">
+        <v>128</v>
+      </c>
+      <c r="D64">
+        <v>2015</v>
+      </c>
+      <c r="E64" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5">
+      <c r="B65" t="s">
+        <v>214</v>
+      </c>
+      <c r="C65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D65">
+        <v>2015</v>
+      </c>
+      <c r="E65" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5">
+      <c r="B66" t="s">
+        <v>214</v>
+      </c>
+      <c r="C66" t="s">
+        <v>130</v>
+      </c>
+      <c r="D66">
+        <v>2015</v>
+      </c>
+      <c r="E66" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5">
+      <c r="B67" t="s">
+        <v>214</v>
+      </c>
+      <c r="C67" t="s">
+        <v>131</v>
+      </c>
+      <c r="D67">
+        <v>2015</v>
+      </c>
+      <c r="E67" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5">
+      <c r="B68" t="s">
+        <v>214</v>
+      </c>
+      <c r="C68" t="s">
+        <v>132</v>
+      </c>
+      <c r="D68">
+        <v>2014</v>
+      </c>
+      <c r="E68" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5">
+      <c r="B69" t="s">
+        <v>214</v>
+      </c>
+      <c r="C69" t="s">
+        <v>133</v>
+      </c>
+      <c r="D69">
+        <v>2014</v>
+      </c>
+      <c r="E69" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5">
+      <c r="B70" t="s">
+        <v>214</v>
+      </c>
+      <c r="C70" t="s">
+        <v>134</v>
+      </c>
+      <c r="D70">
+        <v>2014</v>
+      </c>
+      <c r="E70" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5">
+      <c r="B71" t="s">
+        <v>214</v>
+      </c>
+      <c r="C71" t="s">
+        <v>135</v>
+      </c>
+      <c r="D71">
+        <v>2012</v>
+      </c>
+      <c r="E71" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5">
+      <c r="B72" t="s">
+        <v>214</v>
+      </c>
+      <c r="C72" t="s">
+        <v>136</v>
+      </c>
+      <c r="D72">
+        <v>2011</v>
+      </c>
+      <c r="E72" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5">
+      <c r="B73" t="s">
+        <v>214</v>
+      </c>
+      <c r="C73" t="s">
+        <v>137</v>
+      </c>
+      <c r="D73">
+        <v>2011</v>
+      </c>
+      <c r="E73" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5">
+      <c r="B74" t="s">
+        <v>214</v>
+      </c>
+      <c r="C74" t="s">
+        <v>138</v>
+      </c>
+      <c r="D74">
+        <v>2009</v>
+      </c>
+      <c r="E74" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5">
+      <c r="B75" t="s">
+        <v>214</v>
+      </c>
+      <c r="C75" t="s">
+        <v>139</v>
+      </c>
+      <c r="D75">
+        <v>2009</v>
+      </c>
+      <c r="E75" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5">
+      <c r="B76" t="s">
+        <v>214</v>
+      </c>
+      <c r="C76" t="s">
+        <v>140</v>
+      </c>
+      <c r="D76">
+        <v>2008</v>
+      </c>
+      <c r="E76" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5">
+      <c r="B77" t="s">
+        <v>214</v>
+      </c>
+      <c r="C77" t="s">
+        <v>141</v>
+      </c>
+      <c r="D77">
+        <v>2007</v>
+      </c>
+      <c r="E77" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5">
+      <c r="B78" t="s">
+        <v>214</v>
+      </c>
+      <c r="C78" t="s">
+        <v>142</v>
+      </c>
+      <c r="D78">
+        <v>2006</v>
+      </c>
+      <c r="E78" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -884,10 +2549,100 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C2">
+        <v>2012</v>
+      </c>
+      <c r="D2" t="s">
+        <v>240</v>
+      </c>
+      <c r="E2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F2" t="s">
+        <v>238</v>
+      </c>
+      <c r="G2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3">
+        <v>2012</v>
+      </c>
+      <c r="D3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E3" t="s">
+        <v>233</v>
+      </c>
+      <c r="F3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H54"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -901,114 +2656,226 @@
       <c r="A2" s="2"/>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="3" t="s">
+    <row r="18" spans="1:8">
+      <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="G18" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="G19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="G20" t="s">
         <v>34</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H20" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B38" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B39" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="B42" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B43" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B44" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding papers to preseason review
</commit_message>
<xml_diff>
--- a/refs/litreview/preseason_review.xlsx
+++ b/refs/litreview/preseason_review.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19520" yWindow="0" windowWidth="23700" windowHeight="22500" tabRatio="500"/>
+    <workbookView xWindow="19520" yWindow="0" windowWidth="23700" windowHeight="22500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="preseason_review" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="252">
   <si>
     <t>Search was: You searched for: TOPIC: (preseason  OR pre-season) AND TOPIC: (phenolog*)
 Timespan: All years. Indexes: SCI-EXPANDED, SSCI, A&amp;HCI, CPCI-S, CPCI-SSH, BKCI-S, BKCI-SSH, ESCI, CCR-EXPANDED, IC.</t>
@@ -751,6 +751,33 @@
   </si>
   <si>
     <t>3-mo moving windows beginning the previous fall and ending at the end of the concurrent year, mean daily temperatures were compiled into seasonal growing degree day (GDD) summations and standardized to Z-score values (zero mean, unit SD)</t>
+  </si>
+  <si>
+    <t>Park</t>
+  </si>
+  <si>
+    <t>Herbarium specimens reveal substantial and unexpected variation in phenological sensitivity across the eastern United States</t>
+  </si>
+  <si>
+    <t>Mean March April May Temperature</t>
+  </si>
+  <si>
+    <t>binned data into 4 eco-climate domains</t>
+  </si>
+  <si>
+    <t>Plant phenological synchrony increases under rapid within-spring warming</t>
+  </si>
+  <si>
+    <t>Wang</t>
+  </si>
+  <si>
+    <t>To obtain the effective temperature, we conducted a stepwise regression using the FLD and FFD as dependent variables against the independent variable, i.e., the monthly mean temperature, for each month from November of the previous year to June of the current year. We then performed a stepwise regression for each individual plant. The effective-temperature month was selected by the model with the input P-value of 0.05 and the output P-value of 0.1. To find the most effective period for a phenological event, we then obtained the percentage of the total number of individuals with the effective temperature out of the total number of individuals for each month:</t>
+  </si>
+  <si>
+    <t>We also examined the results for temperature sensitivity for the following four cases: temperature sensitivity was recalculated after the effective temperature and phenological date were detrended, or the effective temperature was redefined as the mean temperature of the 30, 60 or 90 days before the multi-year mean phenological date for each individual. All the results showed results consistent with our original findings</t>
+  </si>
+  <si>
+    <t>This complicated mehtod yeilded: effective temperature of the FLD for most individuals occurred in March and April and that of the FFD for most individuals occurred in February, March and April</t>
   </si>
 </sst>
 </file>
@@ -1305,7 +1332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2557,10 +2584,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2632,6 +2659,55 @@
       </c>
       <c r="F3" t="s">
         <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4" t="s">
+        <v>243</v>
+      </c>
+      <c r="C4">
+        <v>2018</v>
+      </c>
+      <c r="D4" t="s">
+        <v>244</v>
+      </c>
+      <c r="E4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F4" t="s">
+        <v>245</v>
+      </c>
+      <c r="H4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5">
+        <v>2016</v>
+      </c>
+      <c r="D5" t="s">
+        <v>247</v>
+      </c>
+      <c r="E5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F5" t="s">
+        <v>249</v>
+      </c>
+      <c r="G5" t="s">
+        <v>250</v>
+      </c>
+      <c r="H5" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a ref to presaon
</commit_message>
<xml_diff>
--- a/refs/litreview/preseason_review.xlsx
+++ b/refs/litreview/preseason_review.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19520" yWindow="0" windowWidth="23700" windowHeight="22500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1280" yWindow="1420" windowWidth="23700" windowHeight="22500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="preseason_review" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="256">
   <si>
     <t>Search was: You searched for: TOPIC: (preseason  OR pre-season) AND TOPIC: (phenolog*)
 Timespan: All years. Indexes: SCI-EXPANDED, SSCI, A&amp;HCI, CPCI-S, CPCI-SSH, BKCI-S, BKCI-SSH, ESCI, CCR-EXPANDED, IC.</t>
@@ -778,6 +778,18 @@
   </si>
   <si>
     <t>This complicated mehtod yeilded: effective temperature of the FLD for most individuals occurred in March and April and that of the FFD for most individuals occurred in February, March and April</t>
+  </si>
+  <si>
+    <t>Kopp</t>
+  </si>
+  <si>
+    <t>Herbarium records indicate variation in bloom-time sensitivity to temperature across a geographically diverse region</t>
+  </si>
+  <si>
+    <t>mean T for 3 months prior to collection date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For example, if a species had a study-wide mean collection date of June 5, we used temperature data for March, April, and May. </t>
   </si>
 </sst>
 </file>
@@ -2584,10 +2596,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2708,6 +2720,29 @@
       </c>
       <c r="H5" t="s">
         <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" t="s">
+        <v>252</v>
+      </c>
+      <c r="C6">
+        <v>2020</v>
+      </c>
+      <c r="D6" t="s">
+        <v>253</v>
+      </c>
+      <c r="E6" t="s">
+        <v>234</v>
+      </c>
+      <c r="F6" t="s">
+        <v>254</v>
+      </c>
+      <c r="H6" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the lit review so we can look at sensitivity more generally
</commit_message>
<xml_diff>
--- a/refs/litreview/preseason_review.xlsx
+++ b/refs/litreview/preseason_review.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="1420" windowWidth="23700" windowHeight="22500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="5880" yWindow="1360" windowWidth="32300" windowHeight="20520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="preseason_review" sheetId="1" r:id="rId1"/>
     <sheet name="senswindows" sheetId="3" r:id="rId2"/>
-    <sheet name="meta" sheetId="2" r:id="rId3"/>
+    <sheet name="meta" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="572">
   <si>
     <t>Search was: You searched for: TOPIC: (preseason  OR pre-season) AND TOPIC: (phenolog*)
 Timespan: All years. Indexes: SCI-EXPANDED, SSCI, A&amp;HCI, CPCI-S, CPCI-SSH, BKCI-S, BKCI-SSH, ESCI, CCR-EXPANDED, IC.</t>
@@ -790,13 +790,1035 @@
   </si>
   <si>
     <t xml:space="preserve">For example, if a species had a study-wide mean collection date of June 5, we used temperature data for March, April, and May. </t>
+  </si>
+  <si>
+    <t>Satellite-observed decrease in the sensitivity of spring phenology to climate change under high nitrogen deposition</t>
+  </si>
+  <si>
+    <t>Song, ZQ; Fu, YSH; Du, YJ; Li, L; Ouyang, XJ; Ye, WH; Huang, ZL</t>
+  </si>
+  <si>
+    <t>Flowering phenology of a widespread perennial herb shows contrasting responses to global warming between humid and non-humid regions</t>
+  </si>
+  <si>
+    <t>FUNCTIONAL ECOLOGY</t>
+  </si>
+  <si>
+    <t>Gao, MD; Wang, XH; Meng, FD; Liu, Q; Li, XY; Zhang, Y; Piao, SL</t>
+  </si>
+  <si>
+    <t>Three-dimensional change in temperature sensitivity of northern vegetation phenology</t>
+  </si>
+  <si>
+    <t>GLOBAL CHANGE BIOLOGY</t>
+  </si>
+  <si>
+    <t>Menzel, A; Yuan, Y; Matiu, M; Sparks, T; Scheifinger, H; Gehrig, R; Estrella, N</t>
+  </si>
+  <si>
+    <t>Climate change fingerprints in recent European plant phenology</t>
+  </si>
+  <si>
+    <t>AGRICULTURAL AND FOREST METEOROLOGY</t>
+  </si>
+  <si>
+    <t>Wohlfahrt, G; Tomelleri, E; Hammerle, A</t>
+  </si>
+  <si>
+    <t>The urban imprint on plant phenology</t>
+  </si>
+  <si>
+    <t>NATURE ECOLOGY &amp; EVOLUTION</t>
+  </si>
+  <si>
+    <t>Fox, N; Jonsson, AM</t>
+  </si>
+  <si>
+    <t>Climate effects on the onset of flowering in the United Kingdom</t>
+  </si>
+  <si>
+    <t>ENVIRONMENTAL SCIENCES EUROPE</t>
+  </si>
+  <si>
+    <t>Meng, FD; Zhang, LR; Niu, HS; Ji, SN; Zhang, ZH; Wang, Q; Li, BW; Lv, WW; Wang, SP; Duan, JC; Liu, PP; Renzeng, W; Jiang, LL; Luo, CY; Dorji, T; Wang, ZZ; Du, MY</t>
+  </si>
+  <si>
+    <t>Divergent Responses of Community Reproductive and Vegetative Phenology to Warming and Cooling: Asymmetry Versus Symmetry</t>
+  </si>
+  <si>
+    <t>FRONTIERS IN PLANT SCIENCE</t>
+  </si>
+  <si>
+    <t>Helbig, M; Humphreys, ER; Todd, A</t>
+  </si>
+  <si>
+    <t>Contrasting Temperature Sensitivity of CO2 Exchange in Peatlands of the Hudson Bay Lowlands, Canada</t>
+  </si>
+  <si>
+    <t>JOURNAL OF GEOPHYSICAL RESEARCH-BIOGEOSCIENCES</t>
+  </si>
+  <si>
+    <t>ECOLOGY</t>
+  </si>
+  <si>
+    <t>INTERNATIONAL JOURNAL OF BIOMETEOROLOGY</t>
+  </si>
+  <si>
+    <t>ECOLOGY AND EVOLUTION</t>
+  </si>
+  <si>
+    <t>Buchwal, A; Weijers, S; Blok, D; Elberling, B</t>
+  </si>
+  <si>
+    <t>Temperature sensitivity of willow dwarf shrub growth from two distinct High Arctic sites</t>
+  </si>
+  <si>
+    <t>Park, DS; Breckheimer, I; Williams, AC; Law, E; Ellison, AM; Davis, CC</t>
+  </si>
+  <si>
+    <t>PHILOSOPHICAL TRANSACTIONS OF THE ROYAL SOCIETY B-BIOLOGICAL SCIENCES</t>
+  </si>
+  <si>
+    <t>Ji, SN; Classen, AT; Sanders, NJ; He, JS</t>
+  </si>
+  <si>
+    <t>Plant phenological sensitivity to climate change on the Tibetan Plateau and relative to other areas of the world</t>
+  </si>
+  <si>
+    <t>ECOSPHERE</t>
+  </si>
+  <si>
+    <t>INTERNATIONAL JOURNAL OF CLIMATOLOGY</t>
+  </si>
+  <si>
+    <t>Carbognani, M; Tomaselli, M; Petraglia, A</t>
+  </si>
+  <si>
+    <t>Different temperature perception in high-elevation plants: new insight into phenological development and implications for climate change in the alpine tundra</t>
+  </si>
+  <si>
+    <t>OIKOS</t>
+  </si>
+  <si>
+    <t>Meng, FD; Ji, SN; Zhang, ZH; Wang, SP; Duan, JC; Wang, Q; Li, BW; Luo, CY; Jiang, LL; Zhang, LR; Liu, PP; Renzeng, WM; Lv, WW; Wang, ZZ; Tsechoe, D; Du, MY</t>
+  </si>
+  <si>
+    <t>Nonlinear responses of temperature sensitivities of community phenophases to warming and cooling events are mirroring plant functional diversity</t>
+  </si>
+  <si>
+    <t>Wang, HJ; Dai, JH; Rutishauser, T; Gonsamo, A; Wu, CY; Ge, QS</t>
+  </si>
+  <si>
+    <t>Trends and Variability in Temperature Sensitivity of Lilac Flowering Phenology</t>
+  </si>
+  <si>
+    <t>Vitasse, Y; Signarbieux, C; Fu, YSH</t>
+  </si>
+  <si>
+    <t>Global warming leads to more uniform spring phenology across elevations</t>
+  </si>
+  <si>
+    <t>PROCEEDINGS OF THE NATIONAL ACADEMY OF SCIENCES OF THE UNITED STATES OF AMERICA</t>
+  </si>
+  <si>
+    <t>Mo, F; Zhang, J; Wang, J; Cheng, ZG; Sun, GJ; Ren, HX; Zhao, XZ; Cheruiyot, WK; Kavagi, L; Wang, JY; Xiong, YC</t>
+  </si>
+  <si>
+    <t>Phenological evidence from China to address rapid shifts in global flowering times with recent climate change</t>
+  </si>
+  <si>
+    <t>Carroll, CJW; Knapp, AK; Martin, PH</t>
+  </si>
+  <si>
+    <t>Dominant tree species of the Colorado Rockies have divergent physiological and morphological responses to warming</t>
+  </si>
+  <si>
+    <t>FOREST ECOLOGY AND MANAGEMENT</t>
+  </si>
+  <si>
+    <t>Tansey, CJ; Hadfield, JD; Phillimore, AB</t>
+  </si>
+  <si>
+    <t>Estimating the ability of plants to plastically track temperature-mediated shifts in the spring phenological optimum</t>
+  </si>
+  <si>
+    <t>Wang, L; Ning, ZZ; Wang, HJ; Ge, QS</t>
+  </si>
+  <si>
+    <t>Impact of Climate Variability on Flowering Phenology and Its Implications for the Schedule of Blossom Festivals</t>
+  </si>
+  <si>
+    <t>SUSTAINABILITY</t>
+  </si>
+  <si>
+    <t>Prevey, J; Vellend, M; Ruger, N; Hollister, RD; Bjorkman, AD; Myers-Smith, IH; Elmendorf, SC; Clark, K; Cooper, EJ; Elberling, B; Fosaa, AM; Henry, GHR; Hoye, TT; Jonsdottir, IS; Klanderud, K; Levesque, E; Mauritz, M; Molau, U; Natali, SM; Oberbauer, SF; Panchen, ZA; Post, E; Rumpf, SB; Schmidt, NM; Schuur, EAG; Semenchuk, PR; Troxler, T; Welker, JM; Rixen, C</t>
+  </si>
+  <si>
+    <t>Greater temperature sensitivity of plant phenology at colder sites: implications for convergence across northern latitudes</t>
+  </si>
+  <si>
+    <t>Schmid, SF; Stocklin, J; Hamann, E; Kesselring, H</t>
+  </si>
+  <si>
+    <t>High-elevation plants have reduced plasticity in flowering time in response to warming compared to low-elevation congeners</t>
+  </si>
+  <si>
+    <t>BASIC AND APPLIED ECOLOGY</t>
+  </si>
+  <si>
+    <t>Meng, FD; Jiang, LL; Zhang, ZH; Cui, SJ; Duan, JC; Wang, SP; Luo, CY; Wang, Q; Zhou, Y; Li, XE; Zhang, LR; Li, BW; Dorji, T; Li, YN; Du, MY</t>
+  </si>
+  <si>
+    <t>Changes in flowering functional group affect responses of-community phenological sequences to temperature change</t>
+  </si>
+  <si>
+    <t>Panchen, ZA; Gorelick, R</t>
+  </si>
+  <si>
+    <t>Prediction of Arctic plant phenological sensitivity to climate change from historical records</t>
+  </si>
+  <si>
+    <t>Wang, HJ; Rutishauser, T; Tao, ZX; Zhong, SY; Ge, QS; Dai, JH</t>
+  </si>
+  <si>
+    <t>Impacts of global warming on phenology of spring leaf unfolding remain stable in the long run</t>
+  </si>
+  <si>
+    <t>Meng, FD; Zhou, Y; Wang, SP; Duan, JC; Zhang, ZH; Niu, HS; Jiang, LL; Cui, SJ; Li, XE; Luo, CY; Zhang, LR; Wang, Q; Bao, XY; Dorji, T; Li, YN; Du, MY; Zhao, XQ; Zhao, L; Wang, GJ; Inouye, DW</t>
+  </si>
+  <si>
+    <t>Temperature sensitivity thresholds to warming and cooling in phenophases of alpine plants</t>
+  </si>
+  <si>
+    <t>CLIMATIC CHANGE</t>
+  </si>
+  <si>
+    <t>Wang, C; Tang, YH; Chen, J</t>
+  </si>
+  <si>
+    <t>SCIENTIFIC REPORTS</t>
+  </si>
+  <si>
+    <t>Kobayashi, H; Yunus, AP; Nagai, S; Sugiura, K; Kim, Y; Van Dam, B; Nagano, H; Zona, D; Harazono, Y; Bret-Harte, MS; Ichii, K; Ikawa, H; Iwata, H; Oechel, WC; Ueyama, M; Suzuki, R</t>
+  </si>
+  <si>
+    <t>Latitudinal gradient of spruce forest understory and tundra phenology in Alaska as observed from satellite and ground-based data</t>
+  </si>
+  <si>
+    <t>REMOTE SENSING OF ENVIRONMENT</t>
+  </si>
+  <si>
+    <t>He, XY; Xu, S; Xu, WD; Chen, W; Huang, YQ; Wen, H</t>
+  </si>
+  <si>
+    <t>Effects of climate warming on phenological characteristics of urban forest in Shenyang City, China</t>
+  </si>
+  <si>
+    <t>CHINESE GEOGRAPHICAL SCIENCE</t>
+  </si>
+  <si>
+    <t>Zhang, HC; Yuan, WP; Liu, SG; Dong, WJ</t>
+  </si>
+  <si>
+    <t>Divergent responses of leaf phenology to changing temperature among plant species and geographical regions</t>
+  </si>
+  <si>
+    <t>He, ZB; Du, J; Zhao, WZ; Yang, JJ; Chen, LF; Zhu, X; Chang, XX; Liu, H</t>
+  </si>
+  <si>
+    <t>Assessing temperature sensitivity of subalpine shrub phenology in semi-arid mountain regions of China</t>
+  </si>
+  <si>
+    <t>Zhang, HC; Yuan, WP; Liu, SG; Dong, WJ; Fu, Y</t>
+  </si>
+  <si>
+    <t>Sensitivity of flowering phenology to changing temperature in China</t>
+  </si>
+  <si>
+    <t>Marchin, RM; Salk, CF; Hoffmann, WA; Dunn, RR</t>
+  </si>
+  <si>
+    <t>Temperature alone does not explain phenological variation of diverse temperate plants under experimental warming</t>
+  </si>
+  <si>
+    <t>Wang, HJ; Dai, JH; Zheng, JY; Ge, QS</t>
+  </si>
+  <si>
+    <t>Temperature sensitivity of plant phenology in temperate and subtropical regions of China from 1850 to 2009</t>
+  </si>
+  <si>
+    <t>Wang, HJ; Ge, QS; Rutishauser, T; Dai, YX; Dai, JH</t>
+  </si>
+  <si>
+    <t>Parameterization of temperature sensitivity of spring phenology and its application in explaining diverse phenological responses to temperature change</t>
+  </si>
+  <si>
+    <t>ECOLOGICAL INDICATORS</t>
+  </si>
+  <si>
+    <t>Migliavacca, M; Reichstein, M; Richardson, AD; Mahecha, MD; Cremonese, E; Delpierre, N; Galvagno, M; Law, BE; Wohlfahrt, G; Black, TA; Carvalhais, N; Ceccherini, G; Chen, JQ; Gobron, N; Koffi, E; Munger, JW; Perez-Priego, O; Robustelli, M; Tomelleri, E; Cescatti, A</t>
+  </si>
+  <si>
+    <t>Influence of physiological phenology on the seasonal pattern of ecosystem respiration in deciduous forests</t>
+  </si>
+  <si>
+    <t>Liu, LL; Liu, LY; Liang, L; Donnelly, A; Park, I; Schwartz, MD</t>
+  </si>
+  <si>
+    <t>Effects of elevation on spring phenological sensitivity to temperature in Tibetan Plateau grasslands</t>
+  </si>
+  <si>
+    <t>CHINESE SCIENCE BULLETIN</t>
+  </si>
+  <si>
+    <t>Wang, SP; Meng, FD; Duan, JC; Wang, YF; Cui, XY; Piao, SL; Niu, HS; Xu, GP; Luo, CY; Zhang, ZH; Zhu, XX; Shen, MG; Li, YN; Du, MY; Tang, YH; Zhao, XQ; Ciais, P; Kimball, B; Penuelas, J; Janssens, IA; Cui, SJ; Zhao, L; Zhang, FW</t>
+  </si>
+  <si>
+    <t>Asymmetric sensitivity of first flowering date to warming and cooling in alpine plants</t>
+  </si>
+  <si>
+    <t>Hart, R; Salick, J; Ranjitkar, S; Xu, JC</t>
+  </si>
+  <si>
+    <t>Herbarium specimens show contrasting phenological responses to Himalayan climate</t>
+  </si>
+  <si>
+    <t>Dai, JH; Wang, HJ; Ge, QS</t>
+  </si>
+  <si>
+    <t>The spatial pattern of leaf phenology and its response to climate change in China</t>
+  </si>
+  <si>
+    <t>Wang, T; Ottle, C; Peng, SS; Janssens, IA; Lin, X; Poulter, B; Yue, C; Ciais, P</t>
+  </si>
+  <si>
+    <t>The influence of local spring temperature variance on temperature sensitivity of spring phenology</t>
+  </si>
+  <si>
+    <t>Fu, YSH; Campioli, M; Deckmyn, G; Janssens, IA</t>
+  </si>
+  <si>
+    <t>Sensitivity of leaf unfolding to experimental warming in three temperate tree species</t>
+  </si>
+  <si>
+    <t>Chapman, DS</t>
+  </si>
+  <si>
+    <t>Greater phenological sensitivity to temperature on higher Scottish mountains: new insights from remote sensing</t>
+  </si>
+  <si>
+    <t>Bolmgren, K; Vanhoenacker, D; Miller-Rushing, AJ</t>
+  </si>
+  <si>
+    <t>One man, 73 years, and 25 species. Evaluating phenological responses using a lifelong study of first flowering dates</t>
+  </si>
+  <si>
+    <t>Karsai, I; Igartua, E; Casas, AM; Kiss, T; Soos, V; Balla, K; Bedo, Z; Veisz, O</t>
+  </si>
+  <si>
+    <t>Developmental patterns of a large set of barley (Hordeum vulgare) cultivars in response to ambient temperature</t>
+  </si>
+  <si>
+    <t>ANNALS OF APPLIED BIOLOGY</t>
+  </si>
+  <si>
+    <t>Schleip, C; Ankerst, DP; Bock, A; Estrella, N; Menzel, A</t>
+  </si>
+  <si>
+    <t>Comprehensive methodological analysis of long-term changes in phenological extremes in Germany</t>
+  </si>
+  <si>
+    <t>Gunderson, CA; Edwards, NT; Walker, AV; O'Hara, KH; Campion, CM; Hanson, PJ</t>
+  </si>
+  <si>
+    <t>Forest phenology and a warmer climate - growing season extension in relation to climatic provenance</t>
+  </si>
+  <si>
+    <t>journal</t>
+  </si>
+  <si>
+    <t>On 22 Sept 2020 I ran this search on ISI:</t>
+  </si>
+  <si>
+    <t>You searched for: TOPIC: ("temperature sensitivit*") AND TOPIC: (phenolog*) AND TOPIC: (plant*)</t>
+  </si>
+  <si>
+    <t>Timespan: All years. Indexes: SCI-EXPANDED, SSCI, A&amp;HCI, CPCI-S, CPCI-SSH, BKCI-S, BKCI-SSH, ESCI, CCR-EXPANDED, IC.</t>
+  </si>
+  <si>
+    <t>Schleip, C; Rais, A; Menzel, A</t>
+  </si>
+  <si>
+    <t>Bayesian analysis of temperature sensitivity of plant phenology in Germany</t>
+  </si>
+  <si>
+    <t>Rutishauser, T; Luterbacher, J; Defila, C; Frank, D; Wanner, H</t>
+  </si>
+  <si>
+    <t>Swiss spring plant phenology 2007: Extremes, a multi-century perspective, and changes in temperature sensitivity</t>
+  </si>
+  <si>
+    <t>GEOPHYSICAL RESEARCH LETTERS</t>
+  </si>
+  <si>
+    <t>Luo, YQ</t>
+  </si>
+  <si>
+    <t>Terrestrial carbon-cycle feedback to climate warming</t>
+  </si>
+  <si>
+    <t>ANNUAL REVIEW OF ECOLOGY EVOLUTION AND SYSTEMATICS</t>
+  </si>
+  <si>
+    <t>Thompson, R; Clark, RM</t>
+  </si>
+  <si>
+    <t>Spatio-temporal modelling and assessment of within-species phenological variability using thermal time methods</t>
+  </si>
+  <si>
+    <t>Keller, F; Korner, C</t>
+  </si>
+  <si>
+    <t>The role of photoperiodism in alpine plant development</t>
+  </si>
+  <si>
+    <t>ARCTIC ANTARCTIC AND ALPINE RESEARCH</t>
+  </si>
+  <si>
+    <t>It yielded 111 records, I exported them, then deleted any that were about crops, non-spring phenology, non-plant, or were clearly experimental, or were on soil respiration, or were reviews (I did this rather quickly, should check!)</t>
+  </si>
+  <si>
+    <t>What is really shocking is that there are VERY uses of this term before 2012 for plant phenology (21 records in 2011 or before and most were soil or crops).</t>
+  </si>
+  <si>
+    <t>exclude_reason</t>
+  </si>
+  <si>
+    <t>journal title</t>
+  </si>
+  <si>
+    <t>not reviewed closely for some reason, see list below</t>
+  </si>
+  <si>
+    <t>Reasons to exclude:</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>non-plant</t>
+  </si>
+  <si>
+    <t>experiment</t>
+  </si>
+  <si>
+    <t>crop</t>
+  </si>
+  <si>
+    <t>soil temperature sensitivity</t>
+  </si>
+  <si>
+    <t>Nature</t>
+  </si>
+  <si>
+    <t>PNAS</t>
+  </si>
+  <si>
+    <t>PhilTrans</t>
+  </si>
+  <si>
+    <t>IOP Science</t>
+  </si>
+  <si>
+    <t>PEP725 data: "To obtain the effective temperature, we conducted a stepwise regression using
+the FLD and FFD as dependent variables against the independent variable, i.e., the monthly mean temperature,  for each month from November of the previous year to June of the current year. We then performed a stepwise
+regression for each individual plant. The effective-temperature month was selected by the model with the input
+P-value of 0.05 and the output P-value of 0.1." Ugh!</t>
+  </si>
+  <si>
+    <t>backward selection with p-values</t>
+  </si>
+  <si>
+    <t>monthly windows from Nov to June</t>
+  </si>
+  <si>
+    <t>reciprocal transfer</t>
+  </si>
+  <si>
+    <t>Following Fu etal 2015 (Nature), but longer (30 yr) windows</t>
+  </si>
+  <si>
+    <t>Nunavat herbarium records, models with "flowering DOY as the response variable, species as a random effect and May, June, July, and August mean temperatures as fixed effect"</t>
+  </si>
+  <si>
+    <t>picked a May-August month and picked strongest correlation</t>
+  </si>
+  <si>
+    <t>cannot figure it out!</t>
+  </si>
+  <si>
+    <t>NDVI and time-lapse photos</t>
+  </si>
+  <si>
+    <t>really poorly described, who on earth knows</t>
+  </si>
+  <si>
+    <t>"Similar with previous studies (Menzel et al. 2006, Wang et al. 2014a, Wolkovich et al. 2012), the temperature sensitivity was calculated as the slope coefficient of linear regression equations between phenological records and mean preseason temperature"</t>
+  </si>
+  <si>
+    <t>for spring they do Feb-Apr temp</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The whole year in Shenyang was divided into four seasons: winter (from December to February), spring (from
+March to May), summer (from June to August), and autumn (from September to November). The anomaly (the
+difference values between a series recorded temperatures and the average temperature) from 1960 to 2005
+was calculated. The seasonal temperature anomaly, the
+10 year moving mean of the annual average temperature
+and seasonal temperatures were calculated. The linear
+regression equation using a least-squares method was
+obtained (Xia and Zhou, 2002). Coldness index (CI) was
+calculated by the Kira heat index formula: CI= ∑ (5– T).
+Where, T is the yearly or monthly average temperature.
+CI is negative (Xu, 1983; 1986). In this study, T was
+transformed into a ten-day average temperature ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Palatino"/>
+      </rPr>
+      <t>℃</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ten-day) (Xu et al., 2006). Ten tree species with the
+most significant changes were chosen to investigate the
+relationship between phenophase and the mean temperature of each ten-day period. "</t>
+    </r>
+  </si>
+  <si>
+    <t>NDVI "The best singular predictor, one that showed the strongest correlation with SOS/EOS for each site, was selected among a total of 14 possible candidate variables by means of linear regression analysis."</t>
+  </si>
+  <si>
+    <t>searched for highest correlations (by months I think)</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>statisticalsearch (Fu et al 2015)</t>
+  </si>
+  <si>
+    <t>To explore the effects of different periods Snow Cover Duration (SCD) on Start of Season(SOS), "the Spearman’s rank correlation coefficients were used to determine the preseason dominant SCD, which was defined as the period when the highest correlation coefficients occurred between the date of SOS and SCD ahead of SOS with a 1-month step. The maximum range of this period was defined as starting from last October..."</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The maximum range ended on the multiyear average date of SOS (varied spatially from DOY 120-180).</t>
+  </si>
+  <si>
+    <t>1-month step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">statisticalsearch </t>
+  </si>
+  <si>
+    <t>not reported</t>
+  </si>
+  <si>
+    <t>10-day step</t>
+  </si>
+  <si>
+    <t>two months before mean start of growing season</t>
+  </si>
+  <si>
+    <t>start of growing season</t>
+  </si>
+  <si>
+    <t>FFD</t>
+  </si>
+  <si>
+    <t>15-day step</t>
+  </si>
+  <si>
+    <t>LUD</t>
+  </si>
+  <si>
+    <t> mean occurrence of LUD</t>
+  </si>
+  <si>
+    <t>1-day step, up to 120 days before event</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>paper focuses on climate extremes as predictors of growth</t>
+  </si>
+  <si>
+    <t>60 days prior to event</t>
+  </si>
+  <si>
+    <t>wheat harvest date</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>statisticalsearch (I think)</t>
+  </si>
+  <si>
+    <t>0-3 monhts before SOS</t>
+  </si>
+  <si>
+    <t>SOS</t>
+  </si>
+  <si>
+    <t>1 month?</t>
+  </si>
+  <si>
+    <t>no access to paper</t>
+  </si>
+  <si>
+    <t>snow cover end date</t>
+  </si>
+  <si>
+    <t>multiple: 1July, 5 days before LSD</t>
+  </si>
+  <si>
+    <t>leaf senescence date (LSD)</t>
+  </si>
+  <si>
+    <t>unclear</t>
+  </si>
+  <si>
+    <t>15-day steps</t>
+  </si>
+  <si>
+    <t>predefined for precip</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>2 months before SOS</t>
+  </si>
+  <si>
+    <t>statisticalsearch to identify most common (60 days)</t>
+  </si>
+  <si>
+    <t>BBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">predefined </t>
+  </si>
+  <si>
+    <t>median date of budburst or flowering observed over the 2007–2014 observation period for each site</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>one-month steps</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>90 days before event</t>
+  </si>
+  <si>
+    <t>event (SOS or EOS)</t>
+  </si>
+  <si>
+    <t>15-120 days prior</t>
+  </si>
+  <si>
+    <t>mean spring green up</t>
+  </si>
+  <si>
+    <t>3-day step</t>
+  </si>
+  <si>
+    <t>30-150 days before SOS</t>
+  </si>
+  <si>
+    <t>statistical seat</t>
+  </si>
+  <si>
+    <t>20-120 days before event</t>
+  </si>
+  <si>
+    <t>mean date of phenological event</t>
+  </si>
+  <si>
+    <t>statistical search</t>
+  </si>
+  <si>
+    <t>EOS</t>
+  </si>
+  <si>
+    <t>statistical searach</t>
+  </si>
+  <si>
+    <t>0-80 days before event</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>statistical search I think!</t>
+  </si>
+  <si>
+    <t>SOS=start of season</t>
+  </si>
+  <si>
+    <t>Nov-March for precip; preseason window for GDD is unclear</t>
+  </si>
+  <si>
+    <t>after the statistical search, 60 days was used for all sites/species/years</t>
+  </si>
+  <si>
+    <t>EOS = End of Season</t>
+  </si>
+  <si>
+    <t>preseason length = 30-90 days for most pixels</t>
+  </si>
+  <si>
+    <t>separate searches for temp and precip pre-season</t>
+  </si>
+  <si>
+    <r>
+      <t>preceding EOS</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="6"/>
+        <color rgb="FF2A2A2A"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>mean</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF2A2A2A"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> (30-year-average EOS), but after SOS</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="6"/>
+        <color rgb="FF2A2A2A"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>mean</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF2A2A2A"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, with the highest partial correlation coefficient (absolute value) between EOS and temperature, after controlling for precipitation, insolation and SOS</t>
+    </r>
+  </si>
+  <si>
+    <t>yan2020b</t>
+  </si>
+  <si>
+    <t>In brief, the preseason length for the four climatic factors almost ranged between 15 and 90 days</t>
+  </si>
+  <si>
+    <t>dai2019_a</t>
+  </si>
+  <si>
+    <t>see more notes in full_review_guide.xlsx</t>
+  </si>
+  <si>
+    <t>deng2020</t>
+  </si>
+  <si>
+    <t>preseason drought</t>
+  </si>
+  <si>
+    <t>3 months</t>
+  </si>
+  <si>
+    <t>wu2019</t>
+  </si>
+  <si>
+    <t>ghosh2019</t>
+  </si>
+  <si>
+    <t>wang2019</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>2 months</t>
+  </si>
+  <si>
+    <t>estimating peak growing season not start of it</t>
+  </si>
+  <si>
+    <t>du2019</t>
+  </si>
+  <si>
+    <t>They don’t seem to actually say what they used for preseason</t>
+  </si>
+  <si>
+    <t>xia2019</t>
+  </si>
+  <si>
+    <t>spearcorr,parcorr</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>mean SOS</t>
+  </si>
+  <si>
+    <t>yang2019</t>
+  </si>
+  <si>
+    <t>mean max photosynthesis</t>
+  </si>
+  <si>
+    <t>estimating peak phtosynthesis not start of growing season</t>
+  </si>
+  <si>
+    <t>ren2019</t>
+  </si>
+  <si>
+    <t>spearcorr</t>
+  </si>
+  <si>
+    <t>yuan2019</t>
+  </si>
+  <si>
+    <t>correlation coefs</t>
+  </si>
+  <si>
+    <t>16,50,60 prior</t>
+  </si>
+  <si>
+    <t>used different preseasons for different eco-regions</t>
+  </si>
+  <si>
+    <t>deng2019</t>
+  </si>
+  <si>
+    <t>mid-Feb</t>
+  </si>
+  <si>
+    <t>, the TMAX preseason was mainly distributed between mid-February and May of each year</t>
+  </si>
+  <si>
+    <t>guo2019</t>
+  </si>
+  <si>
+    <t>windcrosscorr,pearcorr</t>
+  </si>
+  <si>
+    <t>0-3 months prior</t>
+  </si>
+  <si>
+    <t>GUD</t>
+  </si>
+  <si>
+    <t>regional differnences in preseason correlations</t>
+  </si>
+  <si>
+    <t>mengr2019</t>
+  </si>
+  <si>
+    <t>March?</t>
+  </si>
+  <si>
+    <t>May?</t>
+  </si>
+  <si>
+    <t>hard to tell what they actually used but define spring as March- May</t>
+  </si>
+  <si>
+    <t>Liu2016</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>Average of multi-year EOS</t>
+  </si>
+  <si>
+    <t>1-month steps</t>
+  </si>
+  <si>
+    <t>Spearman’s rank correlation coefficients were used to determine the preseason length that was defined as the period when the highest correlation coefficients occurred between the date of EOS and each of the climatic factors</t>
+  </si>
+  <si>
+    <t>Nguy-Roberts2016</t>
+  </si>
+  <si>
+    <t>models mite-virus risk vs hail event in pre-season</t>
+  </si>
+  <si>
+    <t>Shen2016</t>
+  </si>
+  <si>
+    <t>10-day steps</t>
+  </si>
+  <si>
+    <t>window determined based on average multiyear green-up date, start is variable, they find period with largest partial correlation against greenup</t>
+  </si>
+  <si>
+    <t>Sha2016</t>
+  </si>
+  <si>
+    <t>specifies preseason window in abstract</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>Ge2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pearcorr </t>
+  </si>
+  <si>
+    <t>Start and end variable, comprising 2 months preceeding mean SOS or EOS</t>
+  </si>
+  <si>
+    <t>Shen2015</t>
+  </si>
+  <si>
+    <t>review paper</t>
+  </si>
+  <si>
+    <t>Chen2015</t>
+  </si>
+  <si>
+    <t>measure preseason snowfall</t>
+  </si>
+  <si>
+    <t>did not have access</t>
+  </si>
+  <si>
+    <t>Zhu2015</t>
+  </si>
+  <si>
+    <t>linear reg</t>
+  </si>
+  <si>
+    <t>window determined based on average multiyear green-up date, start is variable, they find period with largest correlation against greenup</t>
+  </si>
+  <si>
+    <t>Wang2015</t>
+  </si>
+  <si>
+    <t>60 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Since the temperature sensitivity of FBD based on different preseason length (e.g., 45 or 90 days) was well correlated with each other (R &gt; 0.8, P &lt; 0.001, data not shown), the preseason period lengths had little impact on the results</t>
+  </si>
+  <si>
+    <t>Yang2015</t>
+  </si>
+  <si>
+    <t>Tang2015</t>
+  </si>
+  <si>
+    <t>Asilo2014</t>
+  </si>
+  <si>
+    <t>does not measure preseason temp</t>
+  </si>
+  <si>
+    <t>Shen2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36 5-day periods from 15 to 120 days </t>
+  </si>
+  <si>
+    <t>moving window prior to SOS, length of window chosen to maximize correlation (r=-1)</t>
+  </si>
+  <si>
+    <t>Xia2014</t>
+  </si>
+  <si>
+    <t>Wainwright2012</t>
+  </si>
+  <si>
+    <t>preseason watering</t>
+  </si>
+  <si>
+    <t>Shen2011</t>
+  </si>
+  <si>
+    <t>Jeong2011</t>
+  </si>
+  <si>
+    <t>Januray</t>
+  </si>
+  <si>
+    <t>4 months</t>
+  </si>
+  <si>
+    <t>they also specify preseason for EOS as june-september</t>
+  </si>
+  <si>
+    <t>Ko2009</t>
+  </si>
+  <si>
+    <t>preseason irrigation</t>
+  </si>
+  <si>
+    <t>Yli-Panula2009</t>
+  </si>
+  <si>
+    <t>12-month moving window</t>
+  </si>
+  <si>
+    <t>Tao2008</t>
+  </si>
+  <si>
+    <t>I have not found how preseason temperature is determined</t>
+  </si>
+  <si>
+    <t>Skjoth2007</t>
+  </si>
+  <si>
+    <t>preseason pollen concentration</t>
+  </si>
+  <si>
+    <t>Berger2006</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -850,6 +1872,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Palatino"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF2E2E2E"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF2A2A2A"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="6"/>
+      <color rgb="FF2A2A2A"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -868,7 +1935,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="67">
+  <cellStyleXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -936,8 +2003,66 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -945,8 +2070,18 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="67">
+  <cellStyles count="125">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -980,6 +2115,35 @@
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1013,6 +2177,35 @@
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1344,11 +2537,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B27" activeCellId="1" sqref="B28 B27"/>
+      <selection pane="bottomRight" activeCell="A53" sqref="A53:XFD78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1646,6 +2839,9 @@
       </c>
     </row>
     <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>481</v>
+      </c>
       <c r="B12" t="s">
         <v>212</v>
       </c>
@@ -1658,8 +2854,20 @@
       <c r="E12" t="s">
         <v>144</v>
       </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L12" t="s">
+        <v>482</v>
+      </c>
     </row>
     <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>483</v>
+      </c>
       <c r="B13" t="s">
         <v>212</v>
       </c>
@@ -1672,8 +2880,20 @@
       <c r="E13" t="s">
         <v>145</v>
       </c>
+      <c r="F13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>485</v>
+      </c>
       <c r="B14" t="s">
         <v>212</v>
       </c>
@@ -1686,8 +2906,20 @@
       <c r="E14" t="s">
         <v>146</v>
       </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" t="s">
+        <v>486</v>
+      </c>
+      <c r="K14" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>488</v>
+      </c>
       <c r="B15" t="s">
         <v>212</v>
       </c>
@@ -1700,8 +2932,23 @@
       <c r="E15" t="s">
         <v>147</v>
       </c>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" t="s">
+        <v>51</v>
+      </c>
+      <c r="J15" t="s">
+        <v>449</v>
+      </c>
     </row>
     <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>489</v>
+      </c>
       <c r="B16" t="s">
         <v>212</v>
       </c>
@@ -1714,8 +2961,17 @@
       <c r="E16" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="17" spans="2:5">
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>490</v>
+      </c>
       <c r="B17" t="s">
         <v>212</v>
       </c>
@@ -1728,8 +2984,29 @@
       <c r="E17" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="18" spans="2:5">
+      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I17" t="s">
+        <v>455</v>
+      </c>
+      <c r="J17" t="s">
+        <v>491</v>
+      </c>
+      <c r="K17" t="s">
+        <v>492</v>
+      </c>
+      <c r="L17" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>494</v>
+      </c>
       <c r="B18" t="s">
         <v>212</v>
       </c>
@@ -1742,8 +3019,20 @@
       <c r="E18" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="19" spans="2:5">
+      <c r="F18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" t="s">
+        <v>34</v>
+      </c>
+      <c r="L18" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>496</v>
+      </c>
       <c r="B19" t="s">
         <v>212</v>
       </c>
@@ -1756,8 +3045,20 @@
       <c r="E19" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="20" spans="2:5">
+      <c r="H19" t="s">
+        <v>497</v>
+      </c>
+      <c r="I19" t="s">
+        <v>498</v>
+      </c>
+      <c r="J19" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>500</v>
+      </c>
       <c r="B20" t="s">
         <v>212</v>
       </c>
@@ -1770,8 +3071,23 @@
       <c r="E20" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="21" spans="2:5">
+      <c r="H20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" t="s">
+        <v>499</v>
+      </c>
+      <c r="J20" t="s">
+        <v>501</v>
+      </c>
+      <c r="L20" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>503</v>
+      </c>
       <c r="B21" t="s">
         <v>212</v>
       </c>
@@ -1784,8 +3100,17 @@
       <c r="E21" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="22" spans="2:5">
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>490</v>
+      </c>
       <c r="B22" t="s">
         <v>212</v>
       </c>
@@ -1798,8 +3123,23 @@
       <c r="E22" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="23" spans="2:5">
+      <c r="F22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" t="s">
+        <v>504</v>
+      </c>
+      <c r="I22" t="s">
+        <v>449</v>
+      </c>
+      <c r="J22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>505</v>
+      </c>
       <c r="B23" t="s">
         <v>212</v>
       </c>
@@ -1812,8 +3152,26 @@
       <c r="E23" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="24" spans="2:5">
+      <c r="F23" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" t="s">
+        <v>506</v>
+      </c>
+      <c r="I23" t="s">
+        <v>507</v>
+      </c>
+      <c r="J23" t="s">
+        <v>439</v>
+      </c>
+      <c r="L23" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="16">
+      <c r="A24" t="s">
+        <v>509</v>
+      </c>
       <c r="B24" t="s">
         <v>212</v>
       </c>
@@ -1826,8 +3184,26 @@
       <c r="E24" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="25" spans="2:5">
+      <c r="F24" t="s">
+        <v>39</v>
+      </c>
+      <c r="H24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I24" t="s">
+        <v>510</v>
+      </c>
+      <c r="J24" t="s">
+        <v>455</v>
+      </c>
+      <c r="L24" s="14" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>512</v>
+      </c>
       <c r="B25" t="s">
         <v>212</v>
       </c>
@@ -1840,8 +3216,26 @@
       <c r="E25" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="26" spans="2:5">
+      <c r="F25" t="s">
+        <v>39</v>
+      </c>
+      <c r="H25" t="s">
+        <v>513</v>
+      </c>
+      <c r="I25" t="s">
+        <v>514</v>
+      </c>
+      <c r="J25" t="s">
+        <v>515</v>
+      </c>
+      <c r="L25" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>517</v>
+      </c>
       <c r="B26" t="s">
         <v>212</v>
       </c>
@@ -1854,8 +3248,23 @@
       <c r="E26" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="27" spans="2:5">
+      <c r="F26" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="J26" t="s">
+        <v>519</v>
+      </c>
+      <c r="L26" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="B27" t="s">
         <v>213</v>
       </c>
@@ -1868,8 +3277,23 @@
       <c r="E27" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="28" spans="2:5">
+      <c r="F27" t="s">
+        <v>417</v>
+      </c>
+      <c r="H27" t="s">
+        <v>418</v>
+      </c>
+      <c r="I27" t="s">
+        <v>419</v>
+      </c>
+      <c r="J27" t="s">
+        <v>420</v>
+      </c>
+      <c r="K27" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="B28" t="s">
         <v>213</v>
       </c>
@@ -1882,8 +3306,23 @@
       <c r="E28" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="29" spans="2:5">
+      <c r="F28" t="s">
+        <v>417</v>
+      </c>
+      <c r="H28" t="s">
+        <v>422</v>
+      </c>
+      <c r="I28" t="s">
+        <v>423</v>
+      </c>
+      <c r="J28" t="s">
+        <v>423</v>
+      </c>
+      <c r="K28" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="B29" t="s">
         <v>213</v>
       </c>
@@ -1896,8 +3335,21 @@
       <c r="E29" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="30" spans="2:5">
+      <c r="F29" t="s">
+        <v>417</v>
+      </c>
+      <c r="H29" t="s">
+        <v>234</v>
+      </c>
+      <c r="I29" t="s">
+        <v>425</v>
+      </c>
+      <c r="J29" t="s">
+        <v>426</v>
+      </c>
+      <c r="L29" s="12"/>
+    </row>
+    <row r="30" spans="1:12">
       <c r="B30" t="s">
         <v>213</v>
       </c>
@@ -1910,8 +3362,20 @@
       <c r="E30" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="31" spans="2:5">
+      <c r="F30" t="s">
+        <v>417</v>
+      </c>
+      <c r="H30" t="s">
+        <v>233</v>
+      </c>
+      <c r="J30" t="s">
+        <v>427</v>
+      </c>
+      <c r="K30" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="B31" t="s">
         <v>213</v>
       </c>
@@ -1924,8 +3388,23 @@
       <c r="E31" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="32" spans="2:5">
+      <c r="F31" t="s">
+        <v>417</v>
+      </c>
+      <c r="H31" t="s">
+        <v>233</v>
+      </c>
+      <c r="I31" t="s">
+        <v>429</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="K31" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="B32" t="s">
         <v>213</v>
       </c>
@@ -1938,8 +3417,14 @@
       <c r="E32" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="33" spans="2:5">
+      <c r="F32" t="s">
+        <v>432</v>
+      </c>
+      <c r="G32" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12">
       <c r="B33" t="s">
         <v>213</v>
       </c>
@@ -1952,8 +3437,20 @@
       <c r="E33" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="34" spans="2:5">
+      <c r="F33" t="s">
+        <v>417</v>
+      </c>
+      <c r="H33" t="s">
+        <v>234</v>
+      </c>
+      <c r="I33" t="s">
+        <v>434</v>
+      </c>
+      <c r="J33" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12">
       <c r="B34" t="s">
         <v>213</v>
       </c>
@@ -1966,8 +3463,26 @@
       <c r="E34" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="35" spans="2:5">
+      <c r="F34" t="s">
+        <v>436</v>
+      </c>
+      <c r="H34" t="s">
+        <v>437</v>
+      </c>
+      <c r="I34" t="s">
+        <v>438</v>
+      </c>
+      <c r="J34" t="s">
+        <v>439</v>
+      </c>
+      <c r="K34" t="s">
+        <v>440</v>
+      </c>
+      <c r="L34" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12">
       <c r="B35" t="s">
         <v>213</v>
       </c>
@@ -1980,8 +3495,14 @@
       <c r="E35" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="36" spans="2:5">
+      <c r="F35" t="s">
+        <v>432</v>
+      </c>
+      <c r="G35" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12">
       <c r="B36" t="s">
         <v>213</v>
       </c>
@@ -1994,8 +3515,20 @@
       <c r="E36" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="37" spans="2:5">
+      <c r="F36" t="s">
+        <v>417</v>
+      </c>
+      <c r="H36" t="s">
+        <v>234</v>
+      </c>
+      <c r="I36" t="s">
+        <v>442</v>
+      </c>
+      <c r="J36" s="10" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12">
       <c r="B37" t="s">
         <v>213</v>
       </c>
@@ -2008,8 +3541,20 @@
       <c r="E37" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="38" spans="2:5">
+      <c r="F37" t="s">
+        <v>417</v>
+      </c>
+      <c r="H37" t="s">
+        <v>234</v>
+      </c>
+      <c r="I37" t="s">
+        <v>443</v>
+      </c>
+      <c r="J37" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12">
       <c r="B38" t="s">
         <v>213</v>
       </c>
@@ -2022,8 +3567,23 @@
       <c r="E38" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="39" spans="2:5">
+      <c r="F38" t="s">
+        <v>417</v>
+      </c>
+      <c r="H38" t="s">
+        <v>233</v>
+      </c>
+      <c r="I38" t="s">
+        <v>445</v>
+      </c>
+      <c r="J38" t="s">
+        <v>427</v>
+      </c>
+      <c r="K38" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12">
       <c r="B39" t="s">
         <v>213</v>
       </c>
@@ -2036,8 +3596,23 @@
       <c r="E39" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="40" spans="2:5">
+      <c r="F39" t="s">
+        <v>417</v>
+      </c>
+      <c r="H39" t="s">
+        <v>447</v>
+      </c>
+      <c r="I39" t="s">
+        <v>448</v>
+      </c>
+      <c r="J39" t="s">
+        <v>449</v>
+      </c>
+      <c r="L39" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12">
       <c r="B40" t="s">
         <v>213</v>
       </c>
@@ -2050,8 +3625,20 @@
       <c r="E40" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="41" spans="2:5">
+      <c r="F40" t="s">
+        <v>417</v>
+      </c>
+      <c r="H40" t="s">
+        <v>234</v>
+      </c>
+      <c r="I40" t="s">
+        <v>450</v>
+      </c>
+      <c r="J40" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12">
       <c r="B41" t="s">
         <v>213</v>
       </c>
@@ -2064,8 +3651,26 @@
       <c r="E41" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="42" spans="2:5">
+      <c r="F41" t="s">
+        <v>436</v>
+      </c>
+      <c r="H41" t="s">
+        <v>451</v>
+      </c>
+      <c r="I41" t="s">
+        <v>434</v>
+      </c>
+      <c r="J41" t="s">
+        <v>452</v>
+      </c>
+      <c r="K41" t="s">
+        <v>446</v>
+      </c>
+      <c r="L41" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12">
       <c r="B42" t="s">
         <v>213</v>
       </c>
@@ -2078,8 +3683,20 @@
       <c r="E42" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="43" spans="2:5">
+      <c r="F42" t="s">
+        <v>436</v>
+      </c>
+      <c r="H42" t="s">
+        <v>453</v>
+      </c>
+      <c r="I42" s="4">
+        <v>43831</v>
+      </c>
+      <c r="J42" s="11" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12">
       <c r="B43" t="s">
         <v>213</v>
       </c>
@@ -2092,8 +3709,23 @@
       <c r="E43" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="44" spans="2:5">
+      <c r="F43" t="s">
+        <v>436</v>
+      </c>
+      <c r="H43" t="s">
+        <v>233</v>
+      </c>
+      <c r="I43" t="s">
+        <v>455</v>
+      </c>
+      <c r="J43" t="s">
+        <v>456</v>
+      </c>
+      <c r="K43" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12">
       <c r="B44" t="s">
         <v>213</v>
       </c>
@@ -2106,8 +3738,14 @@
       <c r="E44" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="45" spans="2:5">
+      <c r="F44" t="s">
+        <v>458</v>
+      </c>
+      <c r="G44" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12">
       <c r="B45" t="s">
         <v>213</v>
       </c>
@@ -2120,8 +3758,23 @@
       <c r="E45" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="46" spans="2:5">
+      <c r="F45" t="s">
+        <v>436</v>
+      </c>
+      <c r="H45" t="s">
+        <v>234</v>
+      </c>
+      <c r="I45" t="s">
+        <v>459</v>
+      </c>
+      <c r="J45" t="s">
+        <v>460</v>
+      </c>
+      <c r="L45" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12">
       <c r="B46" t="s">
         <v>213</v>
       </c>
@@ -2134,8 +3787,26 @@
       <c r="E46" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="47" spans="2:5">
+      <c r="F46" t="s">
+        <v>436</v>
+      </c>
+      <c r="H46" t="s">
+        <v>233</v>
+      </c>
+      <c r="I46" t="s">
+        <v>461</v>
+      </c>
+      <c r="J46" t="s">
+        <v>462</v>
+      </c>
+      <c r="K46" t="s">
+        <v>463</v>
+      </c>
+      <c r="L46" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12">
       <c r="B47" t="s">
         <v>213</v>
       </c>
@@ -2148,8 +3819,26 @@
       <c r="E47" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="48" spans="2:5">
+      <c r="F47" t="s">
+        <v>436</v>
+      </c>
+      <c r="H47" t="s">
+        <v>233</v>
+      </c>
+      <c r="I47" t="s">
+        <v>464</v>
+      </c>
+      <c r="J47" t="s">
+        <v>439</v>
+      </c>
+      <c r="K47" t="s">
+        <v>424</v>
+      </c>
+      <c r="L47" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12">
       <c r="B48" t="s">
         <v>213</v>
       </c>
@@ -2162,8 +3851,23 @@
       <c r="E48" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="49" spans="2:5">
+      <c r="F48" t="s">
+        <v>436</v>
+      </c>
+      <c r="H48" t="s">
+        <v>465</v>
+      </c>
+      <c r="I48" t="s">
+        <v>466</v>
+      </c>
+      <c r="J48" t="s">
+        <v>467</v>
+      </c>
+      <c r="K48" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="B49" t="s">
         <v>213</v>
       </c>
@@ -2176,8 +3880,26 @@
       <c r="E49" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="50" spans="2:5">
+      <c r="F49" t="s">
+        <v>436</v>
+      </c>
+      <c r="H49" t="s">
+        <v>468</v>
+      </c>
+      <c r="I49" t="s">
+        <v>445</v>
+      </c>
+      <c r="J49" t="s">
+        <v>469</v>
+      </c>
+      <c r="K49" t="s">
+        <v>428</v>
+      </c>
+      <c r="L49" s="13" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="B50" t="s">
         <v>213</v>
       </c>
@@ -2190,8 +3912,23 @@
       <c r="E50" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="51" spans="2:5">
+      <c r="F50" t="s">
+        <v>436</v>
+      </c>
+      <c r="H50" t="s">
+        <v>470</v>
+      </c>
+      <c r="I50" t="s">
+        <v>471</v>
+      </c>
+      <c r="J50" t="s">
+        <v>472</v>
+      </c>
+      <c r="K50" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="B51" t="s">
         <v>213</v>
       </c>
@@ -2204,8 +3941,17 @@
       <c r="E51" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="52" spans="2:5">
+      <c r="F51" t="s">
+        <v>458</v>
+      </c>
+      <c r="G51" t="s">
+        <v>441</v>
+      </c>
+      <c r="H51" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="B52" t="s">
         <v>213</v>
       </c>
@@ -2219,7 +3965,10 @@
         <v>184</v>
       </c>
     </row>
-    <row r="53" spans="2:5">
+    <row r="53" spans="1:12">
+      <c r="A53" t="s">
+        <v>521</v>
+      </c>
       <c r="B53" t="s">
         <v>214</v>
       </c>
@@ -2232,8 +3981,29 @@
       <c r="E53" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="54" spans="2:5">
+      <c r="F53" t="s">
+        <v>39</v>
+      </c>
+      <c r="H53" t="s">
+        <v>34</v>
+      </c>
+      <c r="I53" t="s">
+        <v>522</v>
+      </c>
+      <c r="J53" t="s">
+        <v>523</v>
+      </c>
+      <c r="K53" t="s">
+        <v>524</v>
+      </c>
+      <c r="L53" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" t="s">
+        <v>526</v>
+      </c>
       <c r="B54" t="s">
         <v>214</v>
       </c>
@@ -2246,8 +4016,17 @@
       <c r="E54" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="55" spans="2:5">
+      <c r="F54" t="s">
+        <v>23</v>
+      </c>
+      <c r="G54" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" t="s">
+        <v>528</v>
+      </c>
       <c r="B55" t="s">
         <v>214</v>
       </c>
@@ -2260,8 +4039,23 @@
       <c r="E55" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="56" spans="2:5">
+      <c r="F55" t="s">
+        <v>39</v>
+      </c>
+      <c r="H55" t="s">
+        <v>34</v>
+      </c>
+      <c r="K55" t="s">
+        <v>529</v>
+      </c>
+      <c r="L55" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" t="s">
+        <v>531</v>
+      </c>
       <c r="B56" t="s">
         <v>214</v>
       </c>
@@ -2274,8 +4068,23 @@
       <c r="E56" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="57" spans="2:5">
+      <c r="F56" t="s">
+        <v>23</v>
+      </c>
+      <c r="G56" t="s">
+        <v>532</v>
+      </c>
+      <c r="I56" t="s">
+        <v>533</v>
+      </c>
+      <c r="J56" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" t="s">
+        <v>534</v>
+      </c>
       <c r="B57" t="s">
         <v>214</v>
       </c>
@@ -2288,8 +4097,23 @@
       <c r="E57" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="58" spans="2:5">
+      <c r="F57" t="s">
+        <v>39</v>
+      </c>
+      <c r="H57" t="s">
+        <v>535</v>
+      </c>
+      <c r="K57" t="s">
+        <v>492</v>
+      </c>
+      <c r="L57" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" t="s">
+        <v>521</v>
+      </c>
       <c r="B58" t="s">
         <v>214</v>
       </c>
@@ -2302,8 +4126,29 @@
       <c r="E58" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="59" spans="2:5">
+      <c r="F58" t="s">
+        <v>39</v>
+      </c>
+      <c r="H58" t="s">
+        <v>34</v>
+      </c>
+      <c r="I58" t="s">
+        <v>522</v>
+      </c>
+      <c r="J58" t="s">
+        <v>523</v>
+      </c>
+      <c r="K58" t="s">
+        <v>524</v>
+      </c>
+      <c r="L58" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" t="s">
+        <v>537</v>
+      </c>
       <c r="B59" t="s">
         <v>214</v>
       </c>
@@ -2316,8 +4161,17 @@
       <c r="E59" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="60" spans="2:5">
+      <c r="F59" t="s">
+        <v>23</v>
+      </c>
+      <c r="G59" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" t="s">
+        <v>539</v>
+      </c>
       <c r="B60" t="s">
         <v>214</v>
       </c>
@@ -2330,8 +4184,17 @@
       <c r="E60" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="61" spans="2:5">
+      <c r="F60" t="s">
+        <v>23</v>
+      </c>
+      <c r="G60" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" t="s">
+        <v>537</v>
+      </c>
       <c r="B61" t="s">
         <v>214</v>
       </c>
@@ -2344,8 +4207,17 @@
       <c r="E61" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="62" spans="2:5">
+      <c r="F61" t="s">
+        <v>23</v>
+      </c>
+      <c r="G61" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" t="s">
+        <v>542</v>
+      </c>
       <c r="B62" t="s">
         <v>214</v>
       </c>
@@ -2358,8 +4230,23 @@
       <c r="E62" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="63" spans="2:5">
+      <c r="F62" t="s">
+        <v>39</v>
+      </c>
+      <c r="H62" t="s">
+        <v>33</v>
+      </c>
+      <c r="K62" t="s">
+        <v>492</v>
+      </c>
+      <c r="L62" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" t="s">
+        <v>537</v>
+      </c>
       <c r="B63" t="s">
         <v>214</v>
       </c>
@@ -2372,8 +4259,20 @@
       <c r="E63" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="64" spans="2:5">
+      <c r="F63" t="s">
+        <v>39</v>
+      </c>
+      <c r="H63" t="s">
+        <v>543</v>
+      </c>
+      <c r="L63" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" t="s">
+        <v>545</v>
+      </c>
       <c r="B64" t="s">
         <v>214</v>
       </c>
@@ -2386,8 +4285,23 @@
       <c r="E64" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="65" spans="2:5">
+      <c r="F64" t="s">
+        <v>39</v>
+      </c>
+      <c r="H64" t="s">
+        <v>543</v>
+      </c>
+      <c r="K64" t="s">
+        <v>546</v>
+      </c>
+      <c r="L64" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" t="s">
+        <v>545</v>
+      </c>
       <c r="B65" t="s">
         <v>214</v>
       </c>
@@ -2400,8 +4314,20 @@
       <c r="E65" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="66" spans="2:5">
+      <c r="F65" t="s">
+        <v>39</v>
+      </c>
+      <c r="H65" t="s">
+        <v>543</v>
+      </c>
+      <c r="K65" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" t="s">
+        <v>548</v>
+      </c>
       <c r="B66" t="s">
         <v>214</v>
       </c>
@@ -2414,8 +4340,23 @@
       <c r="E66" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="67" spans="2:5">
+      <c r="F66" t="s">
+        <v>23</v>
+      </c>
+      <c r="G66" t="s">
+        <v>532</v>
+      </c>
+      <c r="I66" t="s">
+        <v>455</v>
+      </c>
+      <c r="J66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" t="s">
+        <v>549</v>
+      </c>
       <c r="B67" t="s">
         <v>214</v>
       </c>
@@ -2428,8 +4369,17 @@
       <c r="E67" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="68" spans="2:5">
+      <c r="F67" t="s">
+        <v>23</v>
+      </c>
+      <c r="G67" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" t="s">
+        <v>550</v>
+      </c>
       <c r="B68" t="s">
         <v>214</v>
       </c>
@@ -2442,8 +4392,17 @@
       <c r="E68" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="69" spans="2:5">
+      <c r="F68" t="s">
+        <v>23</v>
+      </c>
+      <c r="G68" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" t="s">
+        <v>552</v>
+      </c>
       <c r="B69" t="s">
         <v>214</v>
       </c>
@@ -2456,8 +4415,23 @@
       <c r="E69" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="70" spans="2:5">
+      <c r="F69" t="s">
+        <v>39</v>
+      </c>
+      <c r="H69" t="s">
+        <v>33</v>
+      </c>
+      <c r="K69" t="s">
+        <v>553</v>
+      </c>
+      <c r="L69" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" t="s">
+        <v>555</v>
+      </c>
       <c r="B70" t="s">
         <v>214</v>
       </c>
@@ -2470,8 +4444,17 @@
       <c r="E70" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="71" spans="2:5">
+      <c r="F70" t="s">
+        <v>23</v>
+      </c>
+      <c r="G70" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" t="s">
+        <v>556</v>
+      </c>
       <c r="B71" t="s">
         <v>214</v>
       </c>
@@ -2484,8 +4467,17 @@
       <c r="E71" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="72" spans="2:5">
+      <c r="F71" t="s">
+        <v>23</v>
+      </c>
+      <c r="G71" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" t="s">
+        <v>558</v>
+      </c>
       <c r="B72" t="s">
         <v>214</v>
       </c>
@@ -2498,8 +4490,17 @@
       <c r="E72" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="73" spans="2:5">
+      <c r="F72" t="s">
+        <v>23</v>
+      </c>
+      <c r="G72" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73" t="s">
+        <v>559</v>
+      </c>
       <c r="B73" t="s">
         <v>214</v>
       </c>
@@ -2512,8 +4513,29 @@
       <c r="E73" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="74" spans="2:5">
+      <c r="F73" t="s">
+        <v>23</v>
+      </c>
+      <c r="G73" t="s">
+        <v>532</v>
+      </c>
+      <c r="I73" t="s">
+        <v>560</v>
+      </c>
+      <c r="J73" t="s">
+        <v>52</v>
+      </c>
+      <c r="K73" t="s">
+        <v>561</v>
+      </c>
+      <c r="L73" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74" t="s">
+        <v>563</v>
+      </c>
       <c r="B74" t="s">
         <v>214</v>
       </c>
@@ -2526,8 +4548,17 @@
       <c r="E74" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="75" spans="2:5">
+      <c r="F74" t="s">
+        <v>23</v>
+      </c>
+      <c r="G74" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75" t="s">
+        <v>565</v>
+      </c>
       <c r="B75" t="s">
         <v>214</v>
       </c>
@@ -2540,8 +4571,20 @@
       <c r="E75" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="76" spans="2:5">
+      <c r="F75" t="s">
+        <v>39</v>
+      </c>
+      <c r="H75" t="s">
+        <v>33</v>
+      </c>
+      <c r="K75" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76" t="s">
+        <v>567</v>
+      </c>
       <c r="B76" t="s">
         <v>214</v>
       </c>
@@ -2554,8 +4597,17 @@
       <c r="E76" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="77" spans="2:5">
+      <c r="F76" t="s">
+        <v>39</v>
+      </c>
+      <c r="L76" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77" t="s">
+        <v>569</v>
+      </c>
       <c r="B77" t="s">
         <v>214</v>
       </c>
@@ -2568,8 +4620,17 @@
       <c r="E77" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="78" spans="2:5">
+      <c r="F77" t="s">
+        <v>23</v>
+      </c>
+      <c r="G77" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78" t="s">
+        <v>571</v>
+      </c>
       <c r="B78" t="s">
         <v>214</v>
       </c>
@@ -2581,6 +4642,12 @@
       </c>
       <c r="E78" t="s">
         <v>210</v>
+      </c>
+      <c r="F78" t="s">
+        <v>23</v>
+      </c>
+      <c r="G78" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2596,15 +4663,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="31.1640625" customWidth="1"/>
+    <col min="9" max="9" width="29.83203125" customWidth="1"/>
+    <col min="10" max="10" width="32.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" s="6" t="s">
         <v>217</v>
       </c>
@@ -2618,19 +4694,25 @@
         <v>4</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>235</v>
       </c>
@@ -2644,16 +4726,19 @@
         <v>240</v>
       </c>
       <c r="E2" t="s">
+        <v>398</v>
+      </c>
+      <c r="G2" t="s">
         <v>234</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>238</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>235</v>
       </c>
@@ -2667,13 +4752,16 @@
         <v>241</v>
       </c>
       <c r="E3" t="s">
+        <v>399</v>
+      </c>
+      <c r="G3" t="s">
         <v>233</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>212</v>
       </c>
@@ -2687,16 +4775,19 @@
         <v>244</v>
       </c>
       <c r="E4" t="s">
+        <v>400</v>
+      </c>
+      <c r="G4" t="s">
         <v>234</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>245</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>212</v>
       </c>
@@ -2710,19 +4801,22 @@
         <v>247</v>
       </c>
       <c r="E5" t="s">
+        <v>324</v>
+      </c>
+      <c r="G5" t="s">
         <v>233</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>249</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>250</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>212</v>
       </c>
@@ -2736,13 +4830,1050 @@
         <v>253</v>
       </c>
       <c r="E6" t="s">
+        <v>279</v>
+      </c>
+      <c r="G6" t="s">
         <v>234</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>254</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C7">
+        <v>2020</v>
+      </c>
+      <c r="D7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E7" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C8">
+        <v>2020</v>
+      </c>
+      <c r="D8" t="s">
+        <v>258</v>
+      </c>
+      <c r="E8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C9">
+        <v>2020</v>
+      </c>
+      <c r="D9" t="s">
+        <v>261</v>
+      </c>
+      <c r="E9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B10" t="s">
+        <v>263</v>
+      </c>
+      <c r="C10">
+        <v>2020</v>
+      </c>
+      <c r="D10" t="s">
+        <v>264</v>
+      </c>
+      <c r="E10" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B11" t="s">
+        <v>266</v>
+      </c>
+      <c r="C11">
+        <v>2019</v>
+      </c>
+      <c r="D11" t="s">
+        <v>267</v>
+      </c>
+      <c r="E11" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>212</v>
+      </c>
+      <c r="B12" t="s">
+        <v>269</v>
+      </c>
+      <c r="C12">
+        <v>2019</v>
+      </c>
+      <c r="D12" t="s">
+        <v>270</v>
+      </c>
+      <c r="E12" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" t="s">
+        <v>272</v>
+      </c>
+      <c r="C13">
+        <v>2019</v>
+      </c>
+      <c r="D13" t="s">
+        <v>273</v>
+      </c>
+      <c r="E13" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B14" t="s">
+        <v>275</v>
+      </c>
+      <c r="C14">
+        <v>2019</v>
+      </c>
+      <c r="D14" t="s">
+        <v>276</v>
+      </c>
+      <c r="E14" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>212</v>
+      </c>
+      <c r="B15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15">
+        <v>2019</v>
+      </c>
+      <c r="D15" t="s">
+        <v>158</v>
+      </c>
+      <c r="E15" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16">
+        <v>2019</v>
+      </c>
+      <c r="D16" t="s">
+        <v>160</v>
+      </c>
+      <c r="E16" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17">
+        <v>2019</v>
+      </c>
+      <c r="D17" t="s">
+        <v>163</v>
+      </c>
+      <c r="E17" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B18" t="s">
+        <v>281</v>
+      </c>
+      <c r="C18">
+        <v>2019</v>
+      </c>
+      <c r="D18" t="s">
+        <v>282</v>
+      </c>
+      <c r="E18" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B19" t="s">
+        <v>283</v>
+      </c>
+      <c r="C19">
+        <v>2019</v>
+      </c>
+      <c r="D19" t="s">
+        <v>244</v>
+      </c>
+      <c r="E19" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B20" t="s">
+        <v>285</v>
+      </c>
+      <c r="C20">
+        <v>2019</v>
+      </c>
+      <c r="D20" t="s">
+        <v>286</v>
+      </c>
+      <c r="E20" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21">
+        <v>2018</v>
+      </c>
+      <c r="D21" t="s">
+        <v>170</v>
+      </c>
+      <c r="E21" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B22" t="s">
+        <v>289</v>
+      </c>
+      <c r="C22">
+        <v>2018</v>
+      </c>
+      <c r="D22" t="s">
+        <v>290</v>
+      </c>
+      <c r="E22" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B23" t="s">
+        <v>292</v>
+      </c>
+      <c r="C23">
+        <v>2018</v>
+      </c>
+      <c r="D23" t="s">
+        <v>293</v>
+      </c>
+      <c r="E23" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B24" t="s">
+        <v>294</v>
+      </c>
+      <c r="C24">
+        <v>2018</v>
+      </c>
+      <c r="D24" t="s">
+        <v>295</v>
+      </c>
+      <c r="E24" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B25" t="s">
+        <v>296</v>
+      </c>
+      <c r="C25">
+        <v>2018</v>
+      </c>
+      <c r="D25" t="s">
+        <v>297</v>
+      </c>
+      <c r="E25" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26">
+        <v>2018</v>
+      </c>
+      <c r="D26" t="s">
+        <v>178</v>
+      </c>
+      <c r="E26" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B27" t="s">
+        <v>299</v>
+      </c>
+      <c r="C27">
+        <v>2017</v>
+      </c>
+      <c r="D27" t="s">
+        <v>300</v>
+      </c>
+      <c r="E27" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B28" t="s">
+        <v>301</v>
+      </c>
+      <c r="C28">
+        <v>2017</v>
+      </c>
+      <c r="D28" t="s">
+        <v>302</v>
+      </c>
+      <c r="E28" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B29" t="s">
+        <v>304</v>
+      </c>
+      <c r="C29">
+        <v>2017</v>
+      </c>
+      <c r="D29" t="s">
+        <v>305</v>
+      </c>
+      <c r="E29" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B30" t="s">
+        <v>306</v>
+      </c>
+      <c r="C30">
+        <v>2017</v>
+      </c>
+      <c r="D30" t="s">
+        <v>307</v>
+      </c>
+      <c r="E30" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B31" t="s">
+        <v>309</v>
+      </c>
+      <c r="C31">
+        <v>2017</v>
+      </c>
+      <c r="D31" t="s">
+        <v>310</v>
+      </c>
+      <c r="E31" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B32" t="s">
+        <v>311</v>
+      </c>
+      <c r="C32">
+        <v>2017</v>
+      </c>
+      <c r="D32" t="s">
+        <v>312</v>
+      </c>
+      <c r="E32" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B33" t="s">
+        <v>314</v>
+      </c>
+      <c r="C33">
+        <v>2017</v>
+      </c>
+      <c r="D33" t="s">
+        <v>315</v>
+      </c>
+      <c r="E33" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="7" customFormat="1">
+      <c r="A34" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="C34" s="7">
+        <v>2017</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="7" customFormat="1">
+      <c r="A35" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="C35" s="7">
+        <v>2017</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="7" customFormat="1">
+      <c r="A36" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="C36" s="7">
+        <v>2016</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="7" customFormat="1">
+      <c r="A37" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="C37" s="7">
+        <v>2016</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="7" customFormat="1">
+      <c r="A38" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="C38" s="7">
+        <v>2016</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="J38" s="7" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="7" customFormat="1">
+      <c r="A39" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="C39" s="7">
+        <v>2016</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="7" customFormat="1">
+      <c r="A40" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="C40" s="7">
+        <v>2015</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="7" customFormat="1">
+      <c r="A41" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="C41" s="7">
+        <v>2015</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B42" t="s">
+        <v>335</v>
+      </c>
+      <c r="C42">
+        <v>2015</v>
+      </c>
+      <c r="D42" t="s">
+        <v>336</v>
+      </c>
+      <c r="E42" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B43" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43">
+        <v>2015</v>
+      </c>
+      <c r="D43" t="s">
+        <v>196</v>
+      </c>
+      <c r="E43" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B44" t="s">
+        <v>337</v>
+      </c>
+      <c r="C44">
+        <v>2015</v>
+      </c>
+      <c r="D44" t="s">
+        <v>338</v>
+      </c>
+      <c r="E44" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B45" t="s">
+        <v>339</v>
+      </c>
+      <c r="C45">
+        <v>2015</v>
+      </c>
+      <c r="D45" t="s">
+        <v>340</v>
+      </c>
+      <c r="E45" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B46" t="s">
+        <v>341</v>
+      </c>
+      <c r="C46">
+        <v>2015</v>
+      </c>
+      <c r="D46" t="s">
+        <v>342</v>
+      </c>
+      <c r="E46" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47">
+        <v>2015</v>
+      </c>
+      <c r="D47" t="s">
+        <v>197</v>
+      </c>
+      <c r="E47" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B48" t="s">
+        <v>344</v>
+      </c>
+      <c r="C48">
+        <v>2015</v>
+      </c>
+      <c r="D48" t="s">
+        <v>345</v>
+      </c>
+      <c r="E48" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B49" t="s">
+        <v>346</v>
+      </c>
+      <c r="C49">
+        <v>2014</v>
+      </c>
+      <c r="D49" t="s">
+        <v>347</v>
+      </c>
+      <c r="E49" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B50" t="s">
+        <v>349</v>
+      </c>
+      <c r="C50">
+        <v>2014</v>
+      </c>
+      <c r="D50" t="s">
+        <v>350</v>
+      </c>
+      <c r="E50" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B51" t="s">
+        <v>351</v>
+      </c>
+      <c r="C51">
+        <v>2014</v>
+      </c>
+      <c r="D51" t="s">
+        <v>352</v>
+      </c>
+      <c r="E51" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B52" t="s">
+        <v>353</v>
+      </c>
+      <c r="C52">
+        <v>2014</v>
+      </c>
+      <c r="D52" t="s">
+        <v>354</v>
+      </c>
+      <c r="E52" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B53" t="s">
+        <v>355</v>
+      </c>
+      <c r="C53">
+        <v>2014</v>
+      </c>
+      <c r="D53" t="s">
+        <v>356</v>
+      </c>
+      <c r="E53" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B54" t="s">
+        <v>357</v>
+      </c>
+      <c r="C54">
+        <v>2013</v>
+      </c>
+      <c r="D54" t="s">
+        <v>358</v>
+      </c>
+      <c r="E54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B55" t="s">
+        <v>359</v>
+      </c>
+      <c r="C55">
+        <v>2013</v>
+      </c>
+      <c r="D55" t="s">
+        <v>360</v>
+      </c>
+      <c r="E55" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B56" t="s">
+        <v>361</v>
+      </c>
+      <c r="C56">
+        <v>2013</v>
+      </c>
+      <c r="D56" t="s">
+        <v>362</v>
+      </c>
+      <c r="E56" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B57" t="s">
+        <v>363</v>
+      </c>
+      <c r="C57">
+        <v>2013</v>
+      </c>
+      <c r="D57" t="s">
+        <v>364</v>
+      </c>
+      <c r="E57" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>212</v>
+      </c>
+      <c r="B58" t="s">
+        <v>366</v>
+      </c>
+      <c r="C58">
+        <v>2012</v>
+      </c>
+      <c r="D58" t="s">
+        <v>367</v>
+      </c>
+      <c r="E58" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>212</v>
+      </c>
+      <c r="B59" t="s">
+        <v>368</v>
+      </c>
+      <c r="C59">
+        <v>2012</v>
+      </c>
+      <c r="D59" t="s">
+        <v>369</v>
+      </c>
+      <c r="E59" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>212</v>
+      </c>
+      <c r="B60" t="s">
+        <v>374</v>
+      </c>
+      <c r="C60">
+        <v>2009</v>
+      </c>
+      <c r="D60" t="s">
+        <v>375</v>
+      </c>
+      <c r="E60" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>212</v>
+      </c>
+      <c r="B61" t="s">
+        <v>376</v>
+      </c>
+      <c r="C61">
+        <v>2008</v>
+      </c>
+      <c r="D61" t="s">
+        <v>377</v>
+      </c>
+      <c r="E61" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>212</v>
+      </c>
+      <c r="B62" t="s">
+        <v>379</v>
+      </c>
+      <c r="C62">
+        <v>2007</v>
+      </c>
+      <c r="D62" t="s">
+        <v>380</v>
+      </c>
+      <c r="E62" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>212</v>
+      </c>
+      <c r="B63" t="s">
+        <v>382</v>
+      </c>
+      <c r="C63">
+        <v>2006</v>
+      </c>
+      <c r="D63" t="s">
+        <v>383</v>
+      </c>
+      <c r="E63" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>212</v>
+      </c>
+      <c r="B64" t="s">
+        <v>384</v>
+      </c>
+      <c r="C64">
+        <v>2003</v>
+      </c>
+      <c r="D64" t="s">
+        <v>385</v>
+      </c>
+      <c r="E64" t="s">
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -2758,10 +5889,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2952,49 +6083,123 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6" t="s">
-        <v>226</v>
+        <v>370</v>
       </c>
       <c r="B42" t="s">
-        <v>227</v>
+        <v>390</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="6" t="s">
-        <v>229</v>
+        <v>389</v>
       </c>
       <c r="B43" t="s">
-        <v>228</v>
+        <v>391</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="6" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B44" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B45" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B46" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="6" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="6"/>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="3" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="6" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="6" t="s">
+        <v>394</v>
+      </c>
+    </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="6" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="6" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="6" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="G56" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
-      <c r="A53" t="s">
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
-      <c r="A54" t="s">
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
         <v>234</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="B64" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="B65" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates from today, pretty close I hope
</commit_message>
<xml_diff>
--- a/refs/litreview/preseason_review.xlsx
+++ b/refs/litreview/preseason_review.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="638">
   <si>
     <t>Search was: You searched for: TOPIC: (preseason  OR pre-season) AND TOPIC: (phenolog*)
 Timespan: All years. Indexes: SCI-EXPANDED, SSCI, A&amp;HCI, CPCI-S, CPCI-SSH, BKCI-S, BKCI-SSH, ESCI, CCR-EXPANDED, IC.</t>
@@ -1264,40 +1264,6 @@
   </si>
   <si>
     <t>for spring they do Feb-Apr temp</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">"The whole year in Shenyang was divided into four seasons: winter (from December to February), spring (from
-March to May), summer (from June to August), and autumn (from September to November). The anomaly (the
-difference values between a series recorded temperatures and the average temperature) from 1960 to 2005
-was calculated. The seasonal temperature anomaly, the
-10 year moving mean of the annual average temperature
-and seasonal temperatures were calculated. The linear
-regression equation using a least-squares method was
-obtained (Xia and Zhou, 2002). Coldness index (CI) was
-calculated by the Kira heat index formula: CI= ∑ (5– T).
-Where, T is the yearly or monthly average temperature.
-CI is negative (Xu, 1983; 1986). In this study, T was
-transformed into a ten-day average temperature ( </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Palatino"/>
-      </rPr>
-      <t>℃</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-ten-day) (Xu et al., 2006). Ten tree species with the
-most significant changes were chosen to investigate the
-relationship between phenophase and the mean temperature of each ten-day period. "</t>
-    </r>
   </si>
   <si>
     <t>NDVI "The best singular predictor, one that showed the strongest correlation with SOS/EOS for each site, was selected among a total of 14 possible candidate variables by means of linear regression analysis."</t>
@@ -1813,12 +1779,463 @@
   <si>
     <t>??</t>
   </si>
+  <si>
+    <t>On 11 October 2020, I pasted in new info from Ailene, Nacho and Dan (and deleted their files).</t>
+  </si>
+  <si>
+    <t>2 months prior to mean date of event</t>
+  </si>
+  <si>
+    <t>mean event</t>
+  </si>
+  <si>
+    <t>10-day step, temperature and precipitation</t>
+  </si>
+  <si>
+    <t>window with largest correlation coefficient selected for statistical search</t>
+  </si>
+  <si>
+    <t>Fu et al 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> both statistical search and predefined</t>
+  </si>
+  <si>
+    <t>July-Aug Air Temperature used for predefined, for search 10-day windows, offset by 1 day</t>
+  </si>
+  <si>
+    <t>monthly and seasonal (2-3 month) temperature used for statistical search</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t> the mean of March, April and May temperatures</t>
+  </si>
+  <si>
+    <t>also tried T range, ΔT, and ΔT/MAT as explanatory variables</t>
+  </si>
+  <si>
+    <t>soil temperature for experiment</t>
+  </si>
+  <si>
+    <t>found that locations with shorter pre-season had weaker Sensitivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snow-free season </t>
+  </si>
+  <si>
+    <t>no months/dates provided for snow-free season</t>
+  </si>
+  <si>
+    <t>starting from the first date on which the 5 cm depth soil temperature remained above 0 °C for five continuous days, and ending on community phenology survey date</t>
+  </si>
+  <si>
+    <t>no months/dates provided for window used</t>
+  </si>
+  <si>
+    <t>response = community phenophase (diversity index); temperature = soil</t>
+  </si>
+  <si>
+    <t>period (with 5 day steps) before the mean FBD for which the Spearman's rank correlation coefficient between FBD and mean temperature was highest during 1963–2013</t>
+  </si>
+  <si>
+    <t>(H. Wang, Zhong, et al., 2017).</t>
+  </si>
+  <si>
+    <t>degree days (days of soil temps &gt;0 degrees C), starting 1Jan, ended on Flowering date</t>
+  </si>
+  <si>
+    <t>MAT and statistical seatch of season (fall, win, spr, sum) preceding flowering that best predicted phenology</t>
+  </si>
+  <si>
+    <t>average temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDD </t>
+  </si>
+  <si>
+    <t>60-day preseason (particular dates varied by site, pre-season ends on average leafout date at each site), tested 45 and 90-day windows as well</t>
+  </si>
+  <si>
+    <t>The start of GDD was fixed at December 1st, January 1st and February 1st; ended on day of leafunfolding</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Separate models were fitted for each month of the year; Models were also fitted with alternative temperature variables based on means over the previous 1–6 months. The optimal temperature averaging period was selected based on minimizing the summed deviance information criteria (DIC) of the GLMMs for each of the 12 months. They found that average of three months prior were  best.</t>
+  </si>
+  <si>
+    <t>60-day window (90 days did not improve fit, 30 days reduced fit)</t>
+  </si>
+  <si>
+    <t>also used statistical search across 12 months</t>
+  </si>
+  <si>
+    <t>crop cultivar</t>
+  </si>
+  <si>
+    <t>no sensitivity</t>
+  </si>
+  <si>
+    <t>simulated anealing algorithm to weight temperature-phenology coherance for mean temperature between Jan and month of phenological event</t>
+  </si>
+  <si>
+    <t>moving window regression for monthly mean temperature</t>
+  </si>
+  <si>
+    <t>1,2,3 month sliding window over 9 month period from mean flowering month</t>
+  </si>
+  <si>
+    <t>parrcorr: 0,1,2 month prior to start of spring</t>
+  </si>
+  <si>
+    <t>aggregated in weeks to study the phenological anomalies from the average</t>
+  </si>
+  <si>
+    <t>Mean T for 30 previous days</t>
+  </si>
+  <si>
+    <t>T during the two preceding months and the month of flowering</t>
+  </si>
+  <si>
+    <t>Jan-March or Feb-April depending on species of interest</t>
+  </si>
+  <si>
+    <t>Nov 1 to certain phenophase</t>
+  </si>
+  <si>
+    <t>25-day moving window from DOY 1-DOY 365</t>
+  </si>
+  <si>
+    <t>CO2 flux not phenology</t>
+  </si>
+  <si>
+    <t>2-mo prior to phenological event</t>
+  </si>
+  <si>
+    <t>45 or 90 days</t>
+  </si>
+  <si>
+    <t>I can't access the article</t>
+  </si>
+  <si>
+    <t>predefined seasonal windows: spring (march-may), winter (December–February), autumn (September–November) and summer (June–August)</t>
+  </si>
+  <si>
+    <t>30 day prior to phenological event</t>
+  </si>
+  <si>
+    <t>2-mo moving window with the later month containing the 27-year average (1982–2008) of spring phenological date for each pixel</t>
+  </si>
+  <si>
+    <t>fixed annual (330-440 days) and monthly (30-40 days) temporal bins</t>
+  </si>
+  <si>
+    <t>either May average temperature, or GDD from Jan 1st until May</t>
+  </si>
+  <si>
+    <t>They calculate the optimal preseason length for each species across years at both low- and high-elevation sites, as the period before themean leaf unfolding across the low- and high-elevation phenology sites, for which the correlation coefficient between leaf-out and air temperature was highest with 5-d steps</t>
+  </si>
+  <si>
+    <t>The preseason climate is calculated in the period preceding greenup from 15 to 120 days with an increment of 3 days</t>
+  </si>
+  <si>
+    <t>?predefined</t>
+  </si>
+  <si>
+    <t>I had a hard time finding what sensitivity window is used</t>
+  </si>
+  <si>
+    <t>The start of the growing season was calculated from the date when 50% of the seedlings at a site had broken dormancy while the end of the growing season was arbitrarily set as September 30th.</t>
+  </si>
+  <si>
+    <t>sliding windows: "the final model included two sliding windows during which mean temperatures predict phenological response...The time window immediately preceding the event (the forcing window) was identical to the best performing temp model for each species."</t>
+  </si>
+  <si>
+    <t>highest Pearson’s correlation with mean temperatures of one month, two months, and three months before the average onset dates</t>
+  </si>
+  <si>
+    <t>The sens-window was defined as either average May–June, June, June–July, or June– August mean monthly temperatures per year, specified separately for each species on the basis of the average time of that phenological event over the period observed across all sites</t>
+  </si>
+  <si>
+    <t>not sure if this would count as predefined, as it changes for species and years</t>
+  </si>
+  <si>
+    <t>I don't find a sens_window</t>
+  </si>
+  <si>
+    <t>I can’t find a sensitivity window nor how was it chosen</t>
+  </si>
+  <si>
+    <t>"The whole year in Shenyang was divided into four seasons: winter (from December to February), spring (from
+March to May), summer (from June to August), and autumn (from September to November). The anomaly (the
+difference values between a series recorded temperatures and the average temperature) from 1960 to 2005
+was calculated. The seasonal temperature anomaly, the
+10 year moving mean of the annual average temperature
+and seasonal temperatures were calculated. The linear
+regression equation using a least-squares method was
+obtained (Xia and Zhou, 2002). Coldness index (CI) was
+calculated by the Kira heat index formula: CI= ∑ (5– T).
+Where, T is the yearly or monthly average temperature.
+CI is negative (Xu, 1983; 1986). In this study, T was
+transformed into a ten-day average temperature ( ℃
+ten-day) (Xu et al., 2006). Ten tree species with the
+most significant changes were chosen to investigate the
+relationship between phenophase and the mean temperature of each ten-day period. "</t>
+  </si>
+  <si>
+    <r>
+      <t>Matsumoto et al. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFA345C9"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2003</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>; Dai et al. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFA345C9"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2013</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The optimal preseason for each species/station defined as the period (with 15‐day steps) before the mean FFD for which the absolute value of Spearman correlation coefficient between FFD and mean temperature was the highest (Dai </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>., </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2013</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>; Fu </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>., </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2015</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>; Wang </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>., </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2017</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> Dai </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>., </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2013</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>; Fu </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>., </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2015</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>; Wang </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>., </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2017</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1878,10 +2295,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Palatino"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF333333"/>
       <name val="Georgia"/>
@@ -1917,6 +2330,64 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2E2E2E"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1C1D1E"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFA345C9"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF1C1D1E"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1935,7 +2406,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="131">
+  <cellStyleXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2067,8 +2538,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2077,17 +2549,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="131" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="131">
+  <cellStyles count="132">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2218,6 +2699,7 @@
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2550,10 +3032,10 @@
   <dimension ref="A1:L78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A53" sqref="A53:XFD78"/>
+      <selection pane="bottomRight" activeCell="A52" sqref="A52:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2852,7 +3334,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B12" t="s">
         <v>212</v>
@@ -2873,12 +3355,12 @@
         <v>34</v>
       </c>
       <c r="L12" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B13" t="s">
         <v>212</v>
@@ -2899,12 +3381,12 @@
         <v>33</v>
       </c>
       <c r="L13" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B14" t="s">
         <v>212</v>
@@ -2922,15 +3404,15 @@
         <v>23</v>
       </c>
       <c r="G14" t="s">
+        <v>484</v>
+      </c>
+      <c r="K14" t="s">
         <v>485</v>
-      </c>
-      <c r="K14" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B15" t="s">
         <v>212</v>
@@ -2954,12 +3436,12 @@
         <v>51</v>
       </c>
       <c r="J15" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B16" t="s">
         <v>212</v>
@@ -2982,7 +3464,7 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B17" t="s">
         <v>212</v>
@@ -3003,21 +3485,21 @@
         <v>34</v>
       </c>
       <c r="I17" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J17" t="s">
+        <v>489</v>
+      </c>
+      <c r="K17" t="s">
         <v>490</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>491</v>
-      </c>
-      <c r="L17" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B18" t="s">
         <v>212</v>
@@ -3038,12 +3520,12 @@
         <v>34</v>
       </c>
       <c r="L18" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B19" t="s">
         <v>212</v>
@@ -3058,18 +3540,18 @@
         <v>151</v>
       </c>
       <c r="H19" t="s">
+        <v>495</v>
+      </c>
+      <c r="I19" t="s">
         <v>496</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>497</v>
-      </c>
-      <c r="J19" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B20" t="s">
         <v>212</v>
@@ -3087,18 +3569,18 @@
         <v>33</v>
       </c>
       <c r="I20" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="J20" t="s">
+        <v>499</v>
+      </c>
+      <c r="L20" t="s">
         <v>500</v>
-      </c>
-      <c r="L20" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B21" t="s">
         <v>212</v>
@@ -3121,7 +3603,7 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B22" t="s">
         <v>212</v>
@@ -3139,10 +3621,10 @@
         <v>39</v>
       </c>
       <c r="H22" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I22" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J22" t="s">
         <v>52</v>
@@ -3150,7 +3632,7 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B23" t="s">
         <v>212</v>
@@ -3168,21 +3650,21 @@
         <v>39</v>
       </c>
       <c r="H23" t="s">
+        <v>504</v>
+      </c>
+      <c r="I23" t="s">
         <v>505</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
+        <v>437</v>
+      </c>
+      <c r="L23" t="s">
         <v>506</v>
-      </c>
-      <c r="J23" t="s">
-        <v>438</v>
-      </c>
-      <c r="L23" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="16">
       <c r="A24" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B24" t="s">
         <v>212</v>
@@ -3203,18 +3685,18 @@
         <v>34</v>
       </c>
       <c r="I24" t="s">
+        <v>508</v>
+      </c>
+      <c r="J24" t="s">
+        <v>453</v>
+      </c>
+      <c r="L24" s="13" t="s">
         <v>509</v>
-      </c>
-      <c r="J24" t="s">
-        <v>454</v>
-      </c>
-      <c r="L24" s="14" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B25" t="s">
         <v>212</v>
@@ -3232,21 +3714,21 @@
         <v>39</v>
       </c>
       <c r="H25" t="s">
+        <v>511</v>
+      </c>
+      <c r="I25" t="s">
         <v>512</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>513</v>
       </c>
-      <c r="J25" t="s">
+      <c r="L25" t="s">
         <v>514</v>
-      </c>
-      <c r="L25" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B26" t="s">
         <v>212</v>
@@ -3267,13 +3749,13 @@
         <v>34</v>
       </c>
       <c r="I26" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="J26" t="s">
         <v>517</v>
       </c>
-      <c r="J26" t="s">
+      <c r="L26" t="s">
         <v>518</v>
-      </c>
-      <c r="L26" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -3290,19 +3772,19 @@
         <v>159</v>
       </c>
       <c r="F27" t="s">
+        <v>415</v>
+      </c>
+      <c r="H27" t="s">
         <v>416</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>417</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>418</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>419</v>
-      </c>
-      <c r="K27" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -3319,19 +3801,19 @@
         <v>160</v>
       </c>
       <c r="F28" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H28" t="s">
+        <v>420</v>
+      </c>
+      <c r="I28" t="s">
         <v>421</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
+        <v>421</v>
+      </c>
+      <c r="K28" t="s">
         <v>422</v>
-      </c>
-      <c r="J28" t="s">
-        <v>422</v>
-      </c>
-      <c r="K28" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -3348,18 +3830,18 @@
         <v>161</v>
       </c>
       <c r="F29" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H29" t="s">
         <v>234</v>
       </c>
       <c r="I29" t="s">
+        <v>423</v>
+      </c>
+      <c r="J29" t="s">
         <v>424</v>
       </c>
-      <c r="J29" t="s">
-        <v>425</v>
-      </c>
-      <c r="L29" s="12"/>
+      <c r="L29" s="11"/>
     </row>
     <row r="30" spans="1:12">
       <c r="B30" t="s">
@@ -3375,16 +3857,16 @@
         <v>162</v>
       </c>
       <c r="F30" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H30" t="s">
         <v>233</v>
       </c>
       <c r="J30" t="s">
+        <v>425</v>
+      </c>
+      <c r="K30" t="s">
         <v>426</v>
-      </c>
-      <c r="K30" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -3401,19 +3883,19 @@
         <v>163</v>
       </c>
       <c r="F31" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H31" t="s">
         <v>233</v>
       </c>
       <c r="I31" t="s">
+        <v>427</v>
+      </c>
+      <c r="J31" s="8" t="s">
         <v>428</v>
       </c>
-      <c r="J31" s="9" t="s">
+      <c r="K31" t="s">
         <v>429</v>
-      </c>
-      <c r="K31" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -3430,10 +3912,10 @@
         <v>164</v>
       </c>
       <c r="F32" t="s">
+        <v>430</v>
+      </c>
+      <c r="G32" t="s">
         <v>431</v>
-      </c>
-      <c r="G32" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="33" spans="2:12">
@@ -3450,16 +3932,16 @@
         <v>165</v>
       </c>
       <c r="F33" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H33" t="s">
         <v>234</v>
       </c>
       <c r="I33" t="s">
+        <v>432</v>
+      </c>
+      <c r="J33" t="s">
         <v>433</v>
-      </c>
-      <c r="J33" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="34" spans="2:12">
@@ -3476,22 +3958,22 @@
         <v>166</v>
       </c>
       <c r="F34" t="s">
+        <v>434</v>
+      </c>
+      <c r="H34" t="s">
         <v>435</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>436</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>437</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>438</v>
       </c>
-      <c r="K34" t="s">
-        <v>439</v>
-      </c>
       <c r="L34" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="35" spans="2:12">
@@ -3508,10 +3990,10 @@
         <v>167</v>
       </c>
       <c r="F35" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G35" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="36" spans="2:12">
@@ -3528,16 +4010,16 @@
         <v>168</v>
       </c>
       <c r="F36" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H36" t="s">
         <v>234</v>
       </c>
       <c r="I36" t="s">
-        <v>441</v>
-      </c>
-      <c r="J36" s="10" t="s">
-        <v>438</v>
+        <v>440</v>
+      </c>
+      <c r="J36" s="9" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="37" spans="2:12">
@@ -3554,16 +4036,16 @@
         <v>169</v>
       </c>
       <c r="F37" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H37" t="s">
         <v>234</v>
       </c>
       <c r="I37" t="s">
+        <v>441</v>
+      </c>
+      <c r="J37" t="s">
         <v>442</v>
-      </c>
-      <c r="J37" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="38" spans="2:12">
@@ -3580,19 +4062,19 @@
         <v>170</v>
       </c>
       <c r="F38" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H38" t="s">
         <v>233</v>
       </c>
       <c r="I38" t="s">
+        <v>443</v>
+      </c>
+      <c r="J38" t="s">
+        <v>425</v>
+      </c>
+      <c r="K38" t="s">
         <v>444</v>
-      </c>
-      <c r="J38" t="s">
-        <v>426</v>
-      </c>
-      <c r="K38" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="39" spans="2:12">
@@ -3609,19 +4091,19 @@
         <v>171</v>
       </c>
       <c r="F39" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H39" t="s">
+        <v>445</v>
+      </c>
+      <c r="I39" t="s">
         <v>446</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>447</v>
       </c>
-      <c r="J39" t="s">
-        <v>448</v>
-      </c>
       <c r="L39" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="40" spans="2:12">
@@ -3638,16 +4120,16 @@
         <v>172</v>
       </c>
       <c r="F40" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H40" t="s">
         <v>234</v>
       </c>
       <c r="I40" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J40" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="41" spans="2:12">
@@ -3664,22 +4146,22 @@
         <v>173</v>
       </c>
       <c r="F41" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H41" t="s">
+        <v>449</v>
+      </c>
+      <c r="I41" t="s">
+        <v>432</v>
+      </c>
+      <c r="J41" t="s">
         <v>450</v>
       </c>
-      <c r="I41" t="s">
-        <v>433</v>
-      </c>
-      <c r="J41" t="s">
-        <v>451</v>
-      </c>
       <c r="K41" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="L41" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="42" spans="2:12">
@@ -3696,16 +4178,16 @@
         <v>174</v>
       </c>
       <c r="F42" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H42" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I42" s="4">
         <v>43831</v>
       </c>
-      <c r="J42" s="11" t="s">
-        <v>453</v>
+      <c r="J42" s="10" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="43" spans="2:12">
@@ -3722,19 +4204,19 @@
         <v>175</v>
       </c>
       <c r="F43" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H43" t="s">
         <v>233</v>
       </c>
       <c r="I43" t="s">
+        <v>453</v>
+      </c>
+      <c r="J43" t="s">
         <v>454</v>
       </c>
-      <c r="J43" t="s">
+      <c r="K43" t="s">
         <v>455</v>
-      </c>
-      <c r="K43" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="44" spans="2:12">
@@ -3751,10 +4233,10 @@
         <v>176</v>
       </c>
       <c r="F44" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G44" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="45" spans="2:12">
@@ -3771,19 +4253,19 @@
         <v>177</v>
       </c>
       <c r="F45" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H45" t="s">
         <v>234</v>
       </c>
       <c r="I45" t="s">
+        <v>457</v>
+      </c>
+      <c r="J45" t="s">
         <v>458</v>
       </c>
-      <c r="J45" t="s">
-        <v>459</v>
-      </c>
       <c r="L45" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="46" spans="2:12">
@@ -3800,22 +4282,22 @@
         <v>178</v>
       </c>
       <c r="F46" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H46" t="s">
         <v>233</v>
       </c>
       <c r="I46" t="s">
+        <v>459</v>
+      </c>
+      <c r="J46" t="s">
         <v>460</v>
       </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
         <v>461</v>
       </c>
-      <c r="K46" t="s">
-        <v>462</v>
-      </c>
       <c r="L46" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="47" spans="2:12">
@@ -3832,22 +4314,22 @@
         <v>179</v>
       </c>
       <c r="F47" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H47" t="s">
         <v>233</v>
       </c>
       <c r="I47" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="J47" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K47" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L47" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="48" spans="2:12">
@@ -3864,19 +4346,19 @@
         <v>180</v>
       </c>
       <c r="F48" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H48" t="s">
+        <v>463</v>
+      </c>
+      <c r="I48" t="s">
         <v>464</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J48" t="s">
         <v>465</v>
       </c>
-      <c r="J48" t="s">
-        <v>466</v>
-      </c>
       <c r="K48" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -3893,22 +4375,22 @@
         <v>181</v>
       </c>
       <c r="F49" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H49" t="s">
+        <v>466</v>
+      </c>
+      <c r="I49" t="s">
+        <v>443</v>
+      </c>
+      <c r="J49" t="s">
         <v>467</v>
       </c>
-      <c r="I49" t="s">
-        <v>444</v>
-      </c>
-      <c r="J49" t="s">
-        <v>468</v>
-      </c>
       <c r="K49" t="s">
-        <v>427</v>
-      </c>
-      <c r="L49" s="13" t="s">
-        <v>479</v>
+        <v>426</v>
+      </c>
+      <c r="L49" s="12" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -3925,19 +4407,19 @@
         <v>182</v>
       </c>
       <c r="F50" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H50" t="s">
+        <v>468</v>
+      </c>
+      <c r="I50" t="s">
         <v>469</v>
       </c>
-      <c r="I50" t="s">
+      <c r="J50" t="s">
         <v>470</v>
       </c>
-      <c r="J50" t="s">
-        <v>471</v>
-      </c>
       <c r="K50" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -3954,32 +4436,47 @@
         <v>183</v>
       </c>
       <c r="F51" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G51" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H51" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12">
-      <c r="B52" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" s="7" customFormat="1">
+      <c r="B52" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="7">
         <v>2017</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="7" t="s">
         <v>184</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="J52" s="7" t="s">
+        <v>573</v>
+      </c>
+      <c r="K52" s="7" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B53" t="s">
         <v>214</v>
@@ -4000,21 +4497,21 @@
         <v>34</v>
       </c>
       <c r="I53" t="s">
+        <v>520</v>
+      </c>
+      <c r="J53" t="s">
         <v>521</v>
       </c>
-      <c r="J53" t="s">
+      <c r="K53" t="s">
         <v>522</v>
       </c>
-      <c r="K53" t="s">
+      <c r="L53" t="s">
         <v>523</v>
-      </c>
-      <c r="L53" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="54" spans="1:12">
       <c r="A54" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B54" t="s">
         <v>214</v>
@@ -4032,12 +4529,12 @@
         <v>23</v>
       </c>
       <c r="G54" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="55" spans="1:12">
       <c r="A55" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B55" t="s">
         <v>214</v>
@@ -4058,15 +4555,15 @@
         <v>34</v>
       </c>
       <c r="K55" t="s">
+        <v>527</v>
+      </c>
+      <c r="L55" t="s">
         <v>528</v>
-      </c>
-      <c r="L55" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="56" spans="1:12">
       <c r="A56" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B56" t="s">
         <v>214</v>
@@ -4084,10 +4581,10 @@
         <v>23</v>
       </c>
       <c r="G56" t="s">
+        <v>530</v>
+      </c>
+      <c r="I56" t="s">
         <v>531</v>
-      </c>
-      <c r="I56" t="s">
-        <v>532</v>
       </c>
       <c r="J56" t="s">
         <v>52</v>
@@ -4095,7 +4592,7 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B57" t="s">
         <v>214</v>
@@ -4113,18 +4610,18 @@
         <v>39</v>
       </c>
       <c r="H57" t="s">
+        <v>533</v>
+      </c>
+      <c r="K57" t="s">
+        <v>490</v>
+      </c>
+      <c r="L57" t="s">
         <v>534</v>
-      </c>
-      <c r="K57" t="s">
-        <v>491</v>
-      </c>
-      <c r="L57" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B58" t="s">
         <v>214</v>
@@ -4145,21 +4642,21 @@
         <v>34</v>
       </c>
       <c r="I58" t="s">
+        <v>520</v>
+      </c>
+      <c r="J58" t="s">
         <v>521</v>
       </c>
-      <c r="J58" t="s">
+      <c r="K58" t="s">
         <v>522</v>
       </c>
-      <c r="K58" t="s">
+      <c r="L58" t="s">
         <v>523</v>
-      </c>
-      <c r="L58" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B59" t="s">
         <v>214</v>
@@ -4177,12 +4674,12 @@
         <v>23</v>
       </c>
       <c r="G59" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="60" spans="1:12">
       <c r="A60" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B60" t="s">
         <v>214</v>
@@ -4200,12 +4697,12 @@
         <v>23</v>
       </c>
       <c r="G60" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="61" spans="1:12">
       <c r="A61" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B61" t="s">
         <v>214</v>
@@ -4223,12 +4720,12 @@
         <v>23</v>
       </c>
       <c r="G61" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="62" spans="1:12">
       <c r="A62" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B62" t="s">
         <v>214</v>
@@ -4249,15 +4746,15 @@
         <v>33</v>
       </c>
       <c r="K62" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="L62" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="63" spans="1:12">
       <c r="A63" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B63" t="s">
         <v>214</v>
@@ -4275,15 +4772,15 @@
         <v>39</v>
       </c>
       <c r="H63" t="s">
+        <v>541</v>
+      </c>
+      <c r="L63" t="s">
         <v>542</v>
-      </c>
-      <c r="L63" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="64" spans="1:12">
       <c r="A64" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B64" t="s">
         <v>214</v>
@@ -4301,18 +4798,18 @@
         <v>39</v>
       </c>
       <c r="H64" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="K64" t="s">
+        <v>544</v>
+      </c>
+      <c r="L64" t="s">
         <v>545</v>
-      </c>
-      <c r="L64" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="65" spans="1:12">
       <c r="A65" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B65" t="s">
         <v>214</v>
@@ -4330,15 +4827,15 @@
         <v>39</v>
       </c>
       <c r="H65" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="K65" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B66" t="s">
         <v>214</v>
@@ -4356,18 +4853,18 @@
         <v>23</v>
       </c>
       <c r="G66" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I66" t="s">
+        <v>453</v>
+      </c>
+      <c r="J66" t="s">
         <v>454</v>
-      </c>
-      <c r="J66" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="67" spans="1:12">
       <c r="A67" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B67" t="s">
         <v>214</v>
@@ -4390,7 +4887,7 @@
     </row>
     <row r="68" spans="1:12">
       <c r="A68" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B68" t="s">
         <v>214</v>
@@ -4408,12 +4905,12 @@
         <v>23</v>
       </c>
       <c r="G68" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="69" spans="1:12">
       <c r="A69" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B69" t="s">
         <v>214</v>
@@ -4434,15 +4931,15 @@
         <v>33</v>
       </c>
       <c r="K69" t="s">
+        <v>551</v>
+      </c>
+      <c r="L69" t="s">
         <v>552</v>
-      </c>
-      <c r="L69" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="70" spans="1:12">
       <c r="A70" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B70" t="s">
         <v>214</v>
@@ -4465,7 +4962,7 @@
     </row>
     <row r="71" spans="1:12">
       <c r="A71" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B71" t="s">
         <v>214</v>
@@ -4483,12 +4980,12 @@
         <v>23</v>
       </c>
       <c r="G71" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="72" spans="1:12">
       <c r="A72" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B72" t="s">
         <v>214</v>
@@ -4506,12 +5003,12 @@
         <v>23</v>
       </c>
       <c r="G72" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="73" spans="1:12">
       <c r="A73" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B73" t="s">
         <v>214</v>
@@ -4529,24 +5026,24 @@
         <v>23</v>
       </c>
       <c r="G73" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I73" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="J73" t="s">
         <v>52</v>
       </c>
       <c r="K73" t="s">
+        <v>559</v>
+      </c>
+      <c r="L73" t="s">
         <v>560</v>
-      </c>
-      <c r="L73" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="74" spans="1:12">
       <c r="A74" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B74" t="s">
         <v>214</v>
@@ -4564,12 +5061,12 @@
         <v>23</v>
       </c>
       <c r="G74" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="75" spans="1:12">
       <c r="A75" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B75" t="s">
         <v>214</v>
@@ -4590,12 +5087,12 @@
         <v>33</v>
       </c>
       <c r="K75" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="76" spans="1:12">
       <c r="A76" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B76" t="s">
         <v>214</v>
@@ -4613,12 +5110,12 @@
         <v>39</v>
       </c>
       <c r="L76" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="77" spans="1:12">
       <c r="A77" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B77" t="s">
         <v>214</v>
@@ -4636,12 +5133,12 @@
         <v>23</v>
       </c>
       <c r="G77" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="78" spans="1:12">
       <c r="A78" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B78" t="s">
         <v>214</v>
@@ -4675,13 +5172,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G40" sqref="G40"/>
+      <selection pane="bottomRight" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4692,1224 +5189,1814 @@
     <col min="10" max="10" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="19" t="s">
         <v>217</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="19" t="s">
         <v>370</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="19" t="s">
         <v>389</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="19" t="s">
         <v>230</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
+      <c r="K1" s="16"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="16">
         <v>2012</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="16" t="s">
         <v>398</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="16" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="16">
         <v>2012</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="16" t="s">
         <v>399</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="16" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="16">
         <v>2018</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="G4" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="J4" t="s">
+      <c r="I4" s="16"/>
+      <c r="J4" s="16" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
+      <c r="K4" s="16"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="16">
         <v>2016</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="16" t="s">
         <v>324</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F5" s="16"/>
+      <c r="G5" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="16" t="s">
         <v>249</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="16" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
+      <c r="K5" s="16"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="16">
         <v>2020</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="G6" t="s">
+      <c r="F6" s="16"/>
+      <c r="G6" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="J6" t="s">
+      <c r="I6" s="16"/>
+      <c r="J6" s="16" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
+      <c r="K6" s="16"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="16">
         <v>2020</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="16" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
+      <c r="F7" s="16"/>
+      <c r="G7" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="16">
         <v>2020</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="16" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
+      <c r="F8" s="16"/>
+      <c r="G8" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>606</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="16">
         <v>2020</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="16" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
+      <c r="F9" s="16"/>
+      <c r="G9" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>607</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="16">
         <v>2020</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="16" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
+      <c r="F10" s="16"/>
+      <c r="G10" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>608</v>
+      </c>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="16">
         <v>2019</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="16" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
+      <c r="F11" s="16"/>
+      <c r="G11" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>609</v>
+      </c>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="16">
         <v>2019</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="16" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
+      <c r="F12" s="16"/>
+      <c r="G12" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>610</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>611</v>
+      </c>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="16" t="s">
         <v>272</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="16">
         <v>2019</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="16" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
+      <c r="F13" s="16"/>
+      <c r="G13" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>612</v>
+      </c>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="16" t="s">
         <v>275</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="16">
         <v>2019</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="16" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
+      <c r="F14" s="19" t="s">
+        <v>397</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>613</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>614</v>
+      </c>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="16">
         <v>2019</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="16" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="7" t="s">
+      <c r="F15" s="16"/>
+      <c r="G15" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>612</v>
+      </c>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+    </row>
+    <row r="16" spans="1:11" s="14" customFormat="1">
+      <c r="A16" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="16">
         <v>2019</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="16" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="7" t="s">
+      <c r="F16" s="16"/>
+      <c r="G16" s="16" t="s">
+        <v>420</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>574</v>
+      </c>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="14" customFormat="1">
+      <c r="A17" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="16">
         <v>2019</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="16" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="7" t="s">
+      <c r="F17" s="16"/>
+      <c r="G17" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>429</v>
+      </c>
+      <c r="I17" s="20"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="20" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="14" customFormat="1">
+      <c r="A18" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="16">
         <v>2019</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="16" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="7" t="s">
+      <c r="F18" s="16"/>
+      <c r="G18" s="16" t="s">
+        <v>577</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>578</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>579</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="14" customFormat="1">
+      <c r="A19" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="16">
         <v>2019</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="16" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="7" t="s">
+      <c r="F19" s="16"/>
+      <c r="G19" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>581</v>
+      </c>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="14" customFormat="1">
+      <c r="A20" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="16">
         <v>2019</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="16" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="7" t="s">
+      <c r="F20" s="16"/>
+      <c r="G20" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>582</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>583</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="14" customFormat="1">
+      <c r="A21" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="16">
         <v>2018</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="16" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="7" t="s">
+      <c r="F21" s="16"/>
+      <c r="G21" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>636</v>
+      </c>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16" t="s">
+        <v>584</v>
+      </c>
+      <c r="K21" s="18" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="14" customFormat="1">
+      <c r="A22" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="16" t="s">
         <v>289</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="16">
         <v>2018</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="16" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="7" t="s">
+      <c r="F22" s="16"/>
+      <c r="G22" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>585</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>586</v>
+      </c>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="14" customFormat="1">
+      <c r="A23" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="16">
         <v>2018</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="16" t="s">
         <v>293</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="16" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="7" t="s">
+      <c r="F23" s="16"/>
+      <c r="G23" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>587</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>588</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="K23" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="14" customFormat="1">
+      <c r="A24" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="16" t="s">
         <v>294</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="16">
         <v>2018</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="16" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="7" t="s">
+      <c r="F24" s="16"/>
+      <c r="G24" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>590</v>
+      </c>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="21" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="1" customFormat="1">
+      <c r="A25" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="23">
         <v>2018</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="23" t="s">
         <v>297</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="23" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="7" t="s">
+      <c r="F25" s="23"/>
+      <c r="G25" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>623</v>
+      </c>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+    </row>
+    <row r="26" spans="1:11" s="1" customFormat="1">
+      <c r="A26" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="23">
         <v>2018</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="23" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="7" t="s">
+      <c r="F26" s="23"/>
+      <c r="G26" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>624</v>
+      </c>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+    </row>
+    <row r="27" spans="1:11" s="1" customFormat="1">
+      <c r="A27" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="23" t="s">
         <v>299</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="23">
         <v>2017</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="23" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="7" t="s">
+      <c r="F27" s="23"/>
+      <c r="G27" s="23" t="s">
+        <v>625</v>
+      </c>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23" t="s">
+        <v>626</v>
+      </c>
+      <c r="K27" s="23"/>
+    </row>
+    <row r="28" spans="1:11" s="1" customFormat="1">
+      <c r="A28" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="23" t="s">
         <v>301</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="23">
         <v>2017</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="23" t="s">
         <v>302</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="23" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="7" t="s">
+      <c r="F28" s="23"/>
+      <c r="G28" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>627</v>
+      </c>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+    </row>
+    <row r="29" spans="1:11" s="1" customFormat="1">
+      <c r="A29" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="23" t="s">
         <v>304</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="23">
         <v>2017</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="23" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="7" t="s">
+      <c r="F29" s="23"/>
+      <c r="G29" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="H29" s="23" t="s">
+        <v>628</v>
+      </c>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+    </row>
+    <row r="30" spans="1:11" s="1" customFormat="1">
+      <c r="A30" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="23" t="s">
         <v>306</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="23">
         <v>2017</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="23" t="s">
         <v>307</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="23" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="7" t="s">
+      <c r="F30" s="23"/>
+      <c r="G30" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="H30" s="23" t="s">
+        <v>629</v>
+      </c>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+    </row>
+    <row r="31" spans="1:11" s="1" customFormat="1">
+      <c r="A31" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="23" t="s">
         <v>309</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="23">
         <v>2017</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="23" t="s">
         <v>310</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="23" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="7" t="s">
+      <c r="F31" s="23"/>
+      <c r="G31" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="H31" s="23" t="s">
+        <v>630</v>
+      </c>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23" t="s">
+        <v>631</v>
+      </c>
+      <c r="K31" s="23"/>
+    </row>
+    <row r="32" spans="1:11" s="1" customFormat="1">
+      <c r="A32" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="23" t="s">
         <v>311</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="23">
         <v>2017</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="23" t="s">
         <v>312</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="23" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="7" t="s">
+      <c r="F32" s="23" t="s">
+        <v>632</v>
+      </c>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23" t="s">
+        <v>633</v>
+      </c>
+      <c r="K32" s="23"/>
+    </row>
+    <row r="33" spans="1:11" s="1" customFormat="1">
+      <c r="A33" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="23" t="s">
         <v>314</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="23">
         <v>2017</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="23" t="s">
         <v>315</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="23" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" s="7" customFormat="1">
-      <c r="A34" s="7" t="s">
+      <c r="F33" s="23" t="s">
+        <v>632</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+    </row>
+    <row r="34" spans="1:11" s="7" customFormat="1">
+      <c r="A34" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="15" t="s">
         <v>316</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="15">
         <v>2017</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="15" t="s">
         <v>317</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="G34" t="s">
+      <c r="F34" s="15"/>
+      <c r="G34" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="H34" s="7" t="s">
+      <c r="H34" s="15" t="s">
         <v>407</v>
       </c>
-      <c r="J34" s="7" t="s">
+      <c r="I34" s="15"/>
+      <c r="J34" s="15" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" s="7" customFormat="1">
-      <c r="A35" s="7" t="s">
+      <c r="K34" s="15"/>
+    </row>
+    <row r="35" spans="1:11" s="7" customFormat="1">
+      <c r="A35" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="15">
         <v>2017</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="15" t="s">
         <v>279</v>
       </c>
-      <c r="G35" t="s">
+      <c r="F35" s="15"/>
+      <c r="G35" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="H35" s="7" t="s">
+      <c r="H35" s="15" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" s="7" customFormat="1">
-      <c r="A36" s="7" t="s">
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+    </row>
+    <row r="36" spans="1:11" s="7" customFormat="1">
+      <c r="A36" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="15">
         <v>2016</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F36" s="15" t="s">
         <v>395</v>
       </c>
-      <c r="G36" s="7" t="s">
+      <c r="G36" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J36" s="7" t="s">
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" s="7" customFormat="1">
-      <c r="A37" s="7" t="s">
+      <c r="K36" s="15"/>
+    </row>
+    <row r="37" spans="1:11" s="7" customFormat="1">
+      <c r="A37" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="15">
         <v>2016</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="15" t="s">
         <v>247</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="F37" s="15"/>
+      <c r="G37" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="H37" s="7" t="s">
+      <c r="H37" s="15" t="s">
         <v>403</v>
       </c>
-      <c r="J37" s="8" t="s">
+      <c r="I37" s="15"/>
+      <c r="J37" s="22" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" s="7" customFormat="1">
-      <c r="A38" s="7" t="s">
+      <c r="K37" s="15"/>
+    </row>
+    <row r="38" spans="1:11" s="7" customFormat="1">
+      <c r="A38" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="15">
         <v>2016</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="G38" s="7" t="s">
-        <v>571</v>
-      </c>
-      <c r="H38" s="7" t="s">
+      <c r="F38" s="15"/>
+      <c r="G38" s="15" t="s">
+        <v>570</v>
+      </c>
+      <c r="H38" s="15" t="s">
         <v>408</v>
       </c>
-      <c r="J38" s="7" t="s">
+      <c r="I38" s="15"/>
+      <c r="J38" s="15" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" s="7" customFormat="1">
-      <c r="A39" s="7" t="s">
+      <c r="K38" s="15"/>
+    </row>
+    <row r="39" spans="1:11" s="7" customFormat="1">
+      <c r="A39" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="15">
         <v>2016</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E39" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="G39" s="7" t="s">
-        <v>571</v>
-      </c>
-      <c r="H39" s="7" t="s">
+      <c r="F39" s="15"/>
+      <c r="G39" s="15" t="s">
+        <v>570</v>
+      </c>
+      <c r="H39" s="15" t="s">
         <v>410</v>
       </c>
-      <c r="J39" s="8" t="s">
+      <c r="I39" s="15"/>
+      <c r="J39" s="22" t="s">
+        <v>634</v>
+      </c>
+      <c r="K39" s="15"/>
+    </row>
+    <row r="40" spans="1:11" s="7" customFormat="1">
+      <c r="A40" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="C40" s="15">
+        <v>2015</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="F40" s="15"/>
+      <c r="G40" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>412</v>
+      </c>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15" t="s">
+        <v>411</v>
+      </c>
+      <c r="K40" s="15"/>
+    </row>
+    <row r="41" spans="1:11" s="7" customFormat="1">
+      <c r="A41" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="C41" s="15">
+        <v>2015</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="F41" s="15"/>
+      <c r="G41" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>414</v>
+      </c>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" s="7" customFormat="1">
-      <c r="A40" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="C40" s="7">
+      <c r="K41" s="15"/>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>335</v>
+      </c>
+      <c r="C42" s="16">
         <v>2015</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>332</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="G40" t="s">
+      <c r="D42" s="16" t="s">
+        <v>336</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="H40" s="7" t="s">
-        <v>412</v>
-      </c>
-      <c r="J40" s="7" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" s="7" customFormat="1">
-      <c r="A41" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="C41" s="7">
+      <c r="H42" s="16" t="s">
+        <v>615</v>
+      </c>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" s="16">
         <v>2015</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="E41" s="7" t="s">
+      <c r="D43" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>616</v>
+      </c>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>337</v>
+      </c>
+      <c r="C44" s="16">
+        <v>2015</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16" t="s">
+        <v>617</v>
+      </c>
+      <c r="K44" s="16"/>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>339</v>
+      </c>
+      <c r="C45" s="16">
+        <v>2015</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H45" s="16" t="s">
+        <v>618</v>
+      </c>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>341</v>
+      </c>
+      <c r="C46" s="16">
+        <v>2015</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>342</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H46" s="16" t="s">
+        <v>619</v>
+      </c>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16"/>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" s="16">
+        <v>2015</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="H47" s="16" t="s">
+        <v>620</v>
+      </c>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="C48" s="16">
+        <v>2015</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>345</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16"/>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>346</v>
+      </c>
+      <c r="C49" s="16">
+        <v>2014</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>348</v>
+      </c>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H49" s="16" t="s">
+        <v>622</v>
+      </c>
+      <c r="I49" s="16"/>
+      <c r="J49" s="16"/>
+      <c r="K49" s="16"/>
+    </row>
+    <row r="50" spans="1:11" s="14" customFormat="1">
+      <c r="A50" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>349</v>
+      </c>
+      <c r="C50" s="16">
+        <v>2014</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H50" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="I50" s="16"/>
+      <c r="J50" s="16"/>
+      <c r="K50" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" s="14" customFormat="1">
+      <c r="A51" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>351</v>
+      </c>
+      <c r="C51" s="16">
+        <v>2014</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>352</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>298</v>
+      </c>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16" t="s">
+        <v>577</v>
+      </c>
+      <c r="H51" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="I51" s="16"/>
+      <c r="J51" s="16"/>
+      <c r="K51" s="16"/>
+    </row>
+    <row r="52" spans="1:11" s="14" customFormat="1">
+      <c r="A52" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>353</v>
+      </c>
+      <c r="C52" s="16">
+        <v>2014</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="H52" s="16" t="s">
+        <v>594</v>
+      </c>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
+      <c r="K52" s="16"/>
+    </row>
+    <row r="53" spans="1:11" s="14" customFormat="1">
+      <c r="A53" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>355</v>
+      </c>
+      <c r="C53" s="16">
+        <v>2014</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>356</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H53" s="16" t="s">
+        <v>595</v>
+      </c>
+      <c r="I53" s="16" t="s">
+        <v>596</v>
+      </c>
+      <c r="J53" s="16"/>
+      <c r="K53" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" s="14" customFormat="1">
+      <c r="A54" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>357</v>
+      </c>
+      <c r="C54" s="16">
+        <v>2013</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>358</v>
+      </c>
+      <c r="E54" s="16" t="s">
         <v>265</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="F54" s="16"/>
+      <c r="G54" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H54" s="16" t="s">
+        <v>595</v>
+      </c>
+      <c r="I54" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="J54" s="16"/>
+      <c r="K54" s="16"/>
+    </row>
+    <row r="55" spans="1:11" s="14" customFormat="1">
+      <c r="A55" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>359</v>
+      </c>
+      <c r="C55" s="16">
+        <v>2013</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="E55" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="H41" s="7" t="s">
-        <v>415</v>
-      </c>
-      <c r="J41" s="7" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="B42" t="s">
-        <v>335</v>
-      </c>
-      <c r="C42">
-        <v>2015</v>
-      </c>
-      <c r="D42" t="s">
-        <v>336</v>
-      </c>
-      <c r="E42" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="B43" t="s">
-        <v>128</v>
-      </c>
-      <c r="C43">
-        <v>2015</v>
-      </c>
-      <c r="D43" t="s">
-        <v>196</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="H55" s="16" t="s">
+        <v>598</v>
+      </c>
+      <c r="I55" s="18" t="s">
+        <v>599</v>
+      </c>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
+    </row>
+    <row r="56" spans="1:11" s="14" customFormat="1">
+      <c r="A56" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="C56" s="16">
+        <v>2013</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="E56" s="16" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="B44" t="s">
-        <v>337</v>
-      </c>
-      <c r="C44">
-        <v>2015</v>
-      </c>
-      <c r="D44" t="s">
-        <v>338</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="F56" s="16"/>
+      <c r="G56" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H56" s="16" t="s">
+        <v>600</v>
+      </c>
+      <c r="I56" s="16" t="s">
+        <v>601</v>
+      </c>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
+    </row>
+    <row r="57" spans="1:11" s="14" customFormat="1">
+      <c r="A57" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>363</v>
+      </c>
+      <c r="C57" s="16">
+        <v>2013</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="F57" s="16" t="s">
+        <v>602</v>
+      </c>
+      <c r="G57" s="16"/>
+      <c r="H57" s="16"/>
+      <c r="I57" s="16"/>
+      <c r="J57" s="16"/>
+      <c r="K57" s="16"/>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="C58" s="16">
+        <v>2012</v>
+      </c>
+      <c r="D58" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="E58" s="16" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="B45" t="s">
-        <v>339</v>
-      </c>
-      <c r="C45">
-        <v>2015</v>
-      </c>
-      <c r="D45" t="s">
-        <v>340</v>
-      </c>
-      <c r="E45" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="B46" t="s">
-        <v>341</v>
-      </c>
-      <c r="C46">
-        <v>2015</v>
-      </c>
-      <c r="D46" t="s">
-        <v>342</v>
-      </c>
-      <c r="E46" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="B47" t="s">
-        <v>129</v>
-      </c>
-      <c r="C47">
-        <v>2015</v>
-      </c>
-      <c r="D47" t="s">
-        <v>197</v>
-      </c>
-      <c r="E47" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="B48" t="s">
-        <v>344</v>
-      </c>
-      <c r="C48">
-        <v>2015</v>
-      </c>
-      <c r="D48" t="s">
-        <v>345</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="F58" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="G58" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="H58" s="16"/>
+      <c r="I58" s="16"/>
+      <c r="J58" s="16"/>
+      <c r="K58" s="16"/>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>368</v>
+      </c>
+      <c r="C59" s="16">
+        <v>2012</v>
+      </c>
+      <c r="D59" s="16" t="s">
+        <v>369</v>
+      </c>
+      <c r="E59" s="16" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="B49" t="s">
-        <v>346</v>
-      </c>
-      <c r="C49">
-        <v>2014</v>
-      </c>
-      <c r="D49" t="s">
-        <v>347</v>
-      </c>
-      <c r="E49" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="B50" t="s">
-        <v>349</v>
-      </c>
-      <c r="C50">
-        <v>2014</v>
-      </c>
-      <c r="D50" t="s">
-        <v>350</v>
-      </c>
-      <c r="E50" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="B51" t="s">
-        <v>351</v>
-      </c>
-      <c r="C51">
-        <v>2014</v>
-      </c>
-      <c r="D51" t="s">
-        <v>352</v>
-      </c>
-      <c r="E51" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="B52" t="s">
-        <v>353</v>
-      </c>
-      <c r="C52">
-        <v>2014</v>
-      </c>
-      <c r="D52" t="s">
-        <v>354</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="F59" s="16" t="s">
+        <v>395</v>
+      </c>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>374</v>
+      </c>
+      <c r="C60" s="16">
+        <v>2009</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="E60" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="H60" s="16" t="s">
+        <v>604</v>
+      </c>
+      <c r="I60" s="16"/>
+      <c r="J60" s="16"/>
+      <c r="K60" s="16"/>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>376</v>
+      </c>
+      <c r="C61" s="16">
+        <v>2008</v>
+      </c>
+      <c r="D61" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="E61" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="H61" s="16" t="s">
+        <v>605</v>
+      </c>
+      <c r="I61" s="16"/>
+      <c r="J61" s="16"/>
+      <c r="K61" s="16"/>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="C62" s="16">
+        <v>2007</v>
+      </c>
+      <c r="D62" s="16" t="s">
+        <v>380</v>
+      </c>
+      <c r="E62" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="F62" s="16" t="s">
+        <v>393</v>
+      </c>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="16"/>
+      <c r="J62" s="16"/>
+      <c r="K62" s="16"/>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="C63" s="16">
+        <v>2006</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>383</v>
+      </c>
+      <c r="E63" s="16" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="B53" t="s">
-        <v>355</v>
-      </c>
-      <c r="C53">
-        <v>2014</v>
-      </c>
-      <c r="D53" t="s">
-        <v>356</v>
-      </c>
-      <c r="E53" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="B54" t="s">
-        <v>357</v>
-      </c>
-      <c r="C54">
-        <v>2013</v>
-      </c>
-      <c r="D54" t="s">
-        <v>358</v>
-      </c>
-      <c r="E54" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="B55" t="s">
-        <v>359</v>
-      </c>
-      <c r="C55">
-        <v>2013</v>
-      </c>
-      <c r="D55" t="s">
-        <v>360</v>
-      </c>
-      <c r="E55" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="B56" t="s">
-        <v>361</v>
-      </c>
-      <c r="C56">
-        <v>2013</v>
-      </c>
-      <c r="D56" t="s">
-        <v>362</v>
-      </c>
-      <c r="E56" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="B57" t="s">
-        <v>363</v>
-      </c>
-      <c r="C57">
-        <v>2013</v>
-      </c>
-      <c r="D57" t="s">
-        <v>364</v>
-      </c>
-      <c r="E57" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" t="s">
+      <c r="F63" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="G63" s="16"/>
+      <c r="H63" s="16"/>
+      <c r="I63" s="16"/>
+      <c r="J63" s="16"/>
+      <c r="K63" s="16"/>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B58" t="s">
-        <v>366</v>
-      </c>
-      <c r="C58">
-        <v>2012</v>
-      </c>
-      <c r="D58" t="s">
-        <v>367</v>
-      </c>
-      <c r="E58" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" t="s">
-        <v>212</v>
-      </c>
-      <c r="B59" t="s">
-        <v>368</v>
-      </c>
-      <c r="C59">
-        <v>2012</v>
-      </c>
-      <c r="D59" t="s">
-        <v>369</v>
-      </c>
-      <c r="E59" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" t="s">
-        <v>212</v>
-      </c>
-      <c r="B60" t="s">
-        <v>374</v>
-      </c>
-      <c r="C60">
-        <v>2009</v>
-      </c>
-      <c r="D60" t="s">
-        <v>375</v>
-      </c>
-      <c r="E60" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" t="s">
-        <v>212</v>
-      </c>
-      <c r="B61" t="s">
-        <v>376</v>
-      </c>
-      <c r="C61">
-        <v>2008</v>
-      </c>
-      <c r="D61" t="s">
-        <v>377</v>
-      </c>
-      <c r="E61" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" t="s">
-        <v>212</v>
-      </c>
-      <c r="B62" t="s">
-        <v>379</v>
-      </c>
-      <c r="C62">
-        <v>2007</v>
-      </c>
-      <c r="D62" t="s">
-        <v>380</v>
-      </c>
-      <c r="E62" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" t="s">
-        <v>212</v>
-      </c>
-      <c r="B63" t="s">
-        <v>382</v>
-      </c>
-      <c r="C63">
-        <v>2006</v>
-      </c>
-      <c r="D63" t="s">
-        <v>383</v>
-      </c>
-      <c r="E63" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" t="s">
-        <v>212</v>
-      </c>
-      <c r="B64" t="s">
+      <c r="B64" s="16" t="s">
         <v>384</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="16">
         <v>2003</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="16" t="s">
         <v>385</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="16" t="s">
         <v>386</v>
       </c>
+      <c r="F64" s="16" t="s">
+        <v>395</v>
+      </c>
+      <c r="G64" s="16"/>
+      <c r="H64" s="16"/>
+      <c r="I64" s="16"/>
+      <c r="J64" s="16"/>
+      <c r="K64" s="16"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K24" r:id="rId1" location="jgrg20969-bib-0050" display="https://agupubs-onlinelibrary-wiley-com.ezp-prod1.hul.harvard.edu/doi/full/10.1002/2017jg004181 - jgrg20969-bib-0050"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -5922,10 +7009,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6233,6 +7320,11 @@
     <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>388</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="2" t="s">
+        <v>571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>